<commit_message>
Removed Sumariser component from Plant.
</commit_message>
<xml_diff>
--- a/Prototypes/Egrandis/EucalyptusValidationData.xlsx
+++ b/Prototypes/Egrandis/EucalyptusValidationData.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ApsimX\Prototypes\Egrandis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="12192" windowHeight="6360" activeTab="2"/>
+    <workbookView xWindow="1080" yWindow="120" windowWidth="12192" windowHeight="6360" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GympieBiomass" sheetId="1" r:id="rId1"/>
@@ -30,7 +35,7 @@
     <definedName name="CYear">#REF!</definedName>
     <definedName name="dlayr">#REF!</definedName>
     <definedName name="e">[1]Sheet2!#REF!</definedName>
-    <definedName name="Irr.times">'[2]IrrSumto7/93'!#REF!</definedName>
+    <definedName name="Irr.times">'[2]93'!#REF!</definedName>
     <definedName name="p">[1]Sheet2!#REF!</definedName>
     <definedName name="PostCost">#REF!</definedName>
     <definedName name="PreCost">#REF!</definedName>
@@ -40,7 +45,7 @@
     <definedName name="SYear">#REF!</definedName>
     <definedName name="WYear">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -224,9 +229,6 @@
     <t>SimulationName</t>
   </si>
   <si>
-    <t>Summariser.AboveGround.Wt</t>
-  </si>
-  <si>
     <t>CoffsHarbour</t>
   </si>
   <si>
@@ -256,15 +258,18 @@
   <si>
     <t>CumulativeLitterFall</t>
   </si>
+  <si>
+    <t>Eucalyptus.AboveGround.Wt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="172" formatCode="0.0"/>
-    <numFmt numFmtId="208" formatCode="[$-C09]dd\-mmm\-yy;@"/>
-    <numFmt numFmtId="211" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="[$-C09]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -319,16 +324,16 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="208" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="211" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -341,13 +346,32 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-AU"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -362,6 +386,7 @@
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -639,6 +664,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -786,32 +812,47 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="140405376"/>
-        <c:axId val="140408704"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="203548392"/>
+        <c:axId val="203539336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="140405376"/>
+        <c:axId val="203548392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140408704"/>
+        <c:crossAx val="203539336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="140408704"/>
+        <c:axId val="203539336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140405376"/>
+        <c:crossAx val="203548392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -832,8 +873,11 @@
           <c:h val="8.3717191601049901E-2"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -845,8 +889,19 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-AU"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -861,6 +916,7 @@
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1138,6 +1194,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1285,32 +1342,47 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="140418048"/>
-        <c:axId val="140436608"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="204315144"/>
+        <c:axId val="204315528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="140418048"/>
+        <c:axId val="204315144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140436608"/>
+        <c:crossAx val="204315528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="140436608"/>
+        <c:axId val="204315528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140418048"/>
+        <c:crossAx val="204315144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1331,8 +1403,11 @@
           <c:h val="8.3717191601049942E-2"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1344,8 +1419,19 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-AU"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -1360,6 +1446,7 @@
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1637,6 +1724,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1784,32 +1872,47 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="143299328"/>
-        <c:axId val="143339904"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="203640200"/>
+        <c:axId val="204061440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="143299328"/>
+        <c:axId val="203640200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143339904"/>
+        <c:crossAx val="204061440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="143339904"/>
+        <c:axId val="204061440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143299328"/>
+        <c:crossAx val="203640200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1830,8 +1933,11 @@
           <c:h val="8.3717191601049942E-2"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1843,8 +1949,19 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-AU"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -1859,6 +1976,7 @@
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2136,6 +2254,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2283,32 +2402,47 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="149377408"/>
-        <c:axId val="149380096"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="203006128"/>
+        <c:axId val="203006520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="149377408"/>
+        <c:axId val="203006128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149380096"/>
+        <c:crossAx val="203006520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149380096"/>
+        <c:axId val="203006520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149377408"/>
+        <c:crossAx val="203006128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2329,8 +2463,11 @@
           <c:h val="8.371719160104997E-2"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2342,12 +2479,24 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-AU"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2634,6 +2783,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2781,32 +2931,47 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="150024960"/>
-        <c:axId val="149444096"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="203008872"/>
+        <c:axId val="203009264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="150024960"/>
+        <c:axId val="203008872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="149444096"/>
+        <c:crossAx val="203009264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="149444096"/>
+        <c:axId val="203009264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150024960"/>
+        <c:crossAx val="203008872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2814,8 +2979,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2827,8 +2995,19 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-AU"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -2843,6 +3022,7 @@
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -3120,6 +3300,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3267,32 +3448,47 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="150729856"/>
-        <c:axId val="150731392"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="203010048"/>
+        <c:axId val="203010440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="150729856"/>
+        <c:axId val="203010048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150731392"/>
+        <c:crossAx val="203010440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="150731392"/>
+        <c:axId val="203010440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150729856"/>
+        <c:crossAx val="203010048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3313,8 +3509,11 @@
           <c:h val="8.3717191601049942E-2"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3326,8 +3525,19 @@
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-AU"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -3342,6 +3552,7 @@
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -3619,6 +3830,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3766,32 +3978,47 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="151693952"/>
-        <c:axId val="151806336"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="203008480"/>
+        <c:axId val="203008088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="151693952"/>
+        <c:axId val="203008480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151806336"/>
+        <c:crossAx val="203008088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="151806336"/>
+        <c:axId val="203008088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151693952"/>
+        <c:crossAx val="203008480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3812,8 +4039,11 @@
           <c:h val="8.371719160104997E-2"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -4039,7 +4269,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Locn"/>
@@ -4076,35 +4306,13 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Sheet2 (2)"/>
-      <sheetName val="Chart2"/>
-      <sheetName val="Chart2 (3)"/>
-      <sheetName val="Chart2 (4)"/>
-      <sheetName val="Chart2 (2)"/>
-      <sheetName val="Chart2 (5)"/>
-      <sheetName val="ClimAct"/>
-      <sheetName val="IrrSumto7/93"/>
-      <sheetName val="Sheet3"/>
-      <sheetName val="Ptn-Mo"/>
-      <sheetName val="ClimAct (2)"/>
+      <sheetName val="93"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4153,7 +4361,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4185,9 +4393,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4219,6 +4428,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4394,11 +4604,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA41"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -4540,11 +4750,11 @@
         <v>0.09</v>
       </c>
       <c r="O2">
-        <f>J2/SUM(H2:J2)</f>
+        <f t="shared" ref="O2:O41" si="1">J2/SUM(H2:J2)</f>
         <v>0.5</v>
       </c>
       <c r="P2">
-        <f>H2+I2</f>
+        <f t="shared" ref="P2:P41" si="2">H2+I2</f>
         <v>4</v>
       </c>
       <c r="R2">
@@ -4572,11 +4782,11 @@
         <v>0.09</v>
       </c>
       <c r="Z2">
-        <f>U2/SUM(S2:U2)</f>
+        <f t="shared" ref="Z2:Z41" si="3">U2/SUM(S2:U2)</f>
         <v>0.5</v>
       </c>
       <c r="AA2">
-        <f>S2+T2</f>
+        <f t="shared" ref="AA2:AA41" si="4">S2+T2</f>
         <v>0.04</v>
       </c>
     </row>
@@ -4594,35 +4804,35 @@
         <v>1.04</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E41" si="1">"Gympie"&amp;IF(C3="Yes","Irrigated","NonIrrigated")&amp;IF(B3="Yes","Fertilised","NonFertilised")</f>
+        <f t="shared" ref="E3:E41" si="5">"Gympie"&amp;IF(C3="Yes","Irrigated","NonIrrigated")&amp;IF(B3="Yes","Fertilised","NonFertilised")</f>
         <v>GympieNonIrrigatedNonFertilised</v>
       </c>
       <c r="F3" s="5">
-        <f t="shared" ref="F3:F41" si="2">DATE(1987,2,4)+365*D3</f>
+        <f t="shared" ref="F3:F41" si="6">DATE(1987,2,4)+365*D3</f>
         <v>32191.599999999999</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G41" si="3">R3*100</f>
+        <f t="shared" ref="G3:G41" si="7">R3*100</f>
         <v>208</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H41" si="4">S3*100</f>
+        <f t="shared" ref="H3:H41" si="8">S3*100</f>
         <v>36</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I41" si="5">T3*100</f>
+        <f t="shared" ref="I3:I41" si="9">T3*100</f>
         <v>9</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J41" si="6">U3*100</f>
+        <f t="shared" ref="J3:J41" si="10">U3*100</f>
         <v>74</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K41" si="7">V3*100</f>
+        <f t="shared" ref="K3:K41" si="11">V3*100</f>
         <v>89</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L41" si="8">W3*100</f>
+        <f t="shared" ref="L3:L41" si="12">W3*100</f>
         <v>119</v>
       </c>
       <c r="M3">
@@ -4632,11 +4842,11 @@
         <v>0.41</v>
       </c>
       <c r="O3">
-        <f>J3/SUM(H3:J3)</f>
+        <f t="shared" si="1"/>
         <v>0.62184873949579833</v>
       </c>
       <c r="P3">
-        <f>H3+I3</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="R3">
@@ -4664,11 +4874,11 @@
         <v>0.41</v>
       </c>
       <c r="Z3">
-        <f>U3/SUM(S3:U3)</f>
+        <f t="shared" si="3"/>
         <v>0.62184873949579833</v>
       </c>
       <c r="AA3">
-        <f>S3+T3</f>
+        <f t="shared" si="4"/>
         <v>0.44999999999999996</v>
       </c>
     </row>
@@ -4686,35 +4896,35 @@
         <v>1.44</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieNonIrrigatedNonFertilised</v>
       </c>
       <c r="F4" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32337.599999999999</v>
       </c>
       <c r="G4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>271</v>
       </c>
       <c r="H4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>62</v>
       </c>
       <c r="I4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="J4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>92</v>
       </c>
       <c r="K4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>99</v>
       </c>
       <c r="L4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>172</v>
       </c>
       <c r="M4">
@@ -4724,11 +4934,11 @@
         <v>1.02</v>
       </c>
       <c r="O4">
-        <f>J4/SUM(H4:J4)</f>
+        <f t="shared" si="1"/>
         <v>0.53488372093023251</v>
       </c>
       <c r="P4">
-        <f>H4+I4</f>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="R4">
@@ -4756,11 +4966,11 @@
         <v>1.02</v>
       </c>
       <c r="Z4">
-        <f>U4/SUM(S4:U4)</f>
+        <f t="shared" si="3"/>
         <v>0.53488372093023251</v>
       </c>
       <c r="AA4">
-        <f>S4+T4</f>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
     </row>
@@ -4778,35 +4988,35 @@
         <v>1.81</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieNonIrrigatedNonFertilised</v>
       </c>
       <c r="F5" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32472.65</v>
       </c>
       <c r="G5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>432</v>
       </c>
       <c r="H5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>182</v>
       </c>
       <c r="I5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>47</v>
       </c>
       <c r="J5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>101</v>
       </c>
       <c r="K5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>102</v>
       </c>
       <c r="L5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>330</v>
       </c>
       <c r="M5">
@@ -4816,11 +5026,11 @@
         <v>0.94</v>
       </c>
       <c r="O5">
-        <f>J5/SUM(H5:J5)</f>
+        <f t="shared" si="1"/>
         <v>0.30606060606060603</v>
       </c>
       <c r="P5">
-        <f>H5+I5</f>
+        <f t="shared" si="2"/>
         <v>229</v>
       </c>
       <c r="R5">
@@ -4848,11 +5058,11 @@
         <v>0.94</v>
       </c>
       <c r="Z5">
-        <f>U5/SUM(S5:U5)</f>
+        <f t="shared" si="3"/>
         <v>0.30606060606060609</v>
       </c>
       <c r="AA5">
-        <f>S5+T5</f>
+        <f t="shared" si="4"/>
         <v>2.29</v>
       </c>
     </row>
@@ -4870,35 +5080,35 @@
         <v>2.4</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieNonIrrigatedNonFertilised</v>
       </c>
       <c r="F6" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32688</v>
       </c>
       <c r="G6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>818</v>
       </c>
       <c r="H6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>401</v>
       </c>
       <c r="I6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>91</v>
       </c>
       <c r="J6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>174</v>
       </c>
       <c r="K6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>152</v>
       </c>
       <c r="L6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>666</v>
       </c>
       <c r="M6">
@@ -4908,11 +5118,11 @@
         <v>1.24</v>
       </c>
       <c r="O6">
-        <f>J6/SUM(H6:J6)</f>
+        <f t="shared" si="1"/>
         <v>0.26126126126126126</v>
       </c>
       <c r="P6">
-        <f>H6+I6</f>
+        <f t="shared" si="2"/>
         <v>492</v>
       </c>
       <c r="R6">
@@ -4940,11 +5150,11 @@
         <v>1.24</v>
       </c>
       <c r="Z6">
-        <f>U6/SUM(S6:U6)</f>
+        <f t="shared" si="3"/>
         <v>0.26126126126126126</v>
       </c>
       <c r="AA6">
-        <f>S6+T6</f>
+        <f t="shared" si="4"/>
         <v>4.92</v>
       </c>
     </row>
@@ -4962,35 +5172,35 @@
         <v>3.1</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieNonIrrigatedNonFertilised</v>
       </c>
       <c r="F7" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32943.5</v>
       </c>
       <c r="G7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1443</v>
       </c>
       <c r="H7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>923</v>
       </c>
       <c r="I7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>196</v>
       </c>
       <c r="J7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>175</v>
       </c>
       <c r="K7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>149</v>
       </c>
       <c r="L7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1294</v>
       </c>
       <c r="M7">
@@ -5000,11 +5210,11 @@
         <v>0.9511586455971146</v>
       </c>
       <c r="O7">
-        <f>J7/SUM(H7:J7)</f>
+        <f t="shared" si="1"/>
         <v>0.13523956723338484</v>
       </c>
       <c r="P7">
-        <f>H7+I7</f>
+        <f t="shared" si="2"/>
         <v>1119</v>
       </c>
       <c r="R7">
@@ -5032,11 +5242,11 @@
         <v>0.9511586455971146</v>
       </c>
       <c r="Z7">
-        <f>U7/SUM(S7:U7)</f>
+        <f t="shared" si="3"/>
         <v>0.13523956723338484</v>
       </c>
       <c r="AA7">
-        <f>S7+T7</f>
+        <f t="shared" si="4"/>
         <v>11.190000000000001</v>
       </c>
     </row>
@@ -5054,35 +5264,35 @@
         <v>3.6</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieNonIrrigatedNonFertilised</v>
       </c>
       <c r="F8" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>33126</v>
       </c>
       <c r="G8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1847</v>
       </c>
       <c r="H8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1162</v>
       </c>
       <c r="I8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>242</v>
       </c>
       <c r="J8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>266</v>
       </c>
       <c r="K8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>177</v>
       </c>
       <c r="L8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1670</v>
       </c>
       <c r="M8">
@@ -5092,11 +5302,11 @@
         <v>1.0711441730922997</v>
       </c>
       <c r="O8">
-        <f>J8/SUM(H8:J8)</f>
+        <f t="shared" si="1"/>
         <v>0.15928143712574849</v>
       </c>
       <c r="P8">
-        <f>H8+I8</f>
+        <f t="shared" si="2"/>
         <v>1404</v>
       </c>
       <c r="R8">
@@ -5124,11 +5334,11 @@
         <v>1.0711441730922997</v>
       </c>
       <c r="Z8">
-        <f>U8/SUM(S8:U8)</f>
+        <f t="shared" si="3"/>
         <v>0.15928143712574852</v>
       </c>
       <c r="AA8">
-        <f>S8+T8</f>
+        <f t="shared" si="4"/>
         <v>14.04</v>
       </c>
     </row>
@@ -5146,35 +5356,35 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieNonIrrigatedNonFertilised</v>
       </c>
       <c r="F9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>33308.5</v>
       </c>
       <c r="G9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2287</v>
       </c>
       <c r="H9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1425</v>
       </c>
       <c r="I9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>291</v>
       </c>
       <c r="J9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>367</v>
       </c>
       <c r="K9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>204</v>
       </c>
       <c r="L9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2083</v>
       </c>
       <c r="M9">
@@ -5184,11 +5394,11 @@
         <v>1.2346715502656165</v>
       </c>
       <c r="O9">
-        <f>J9/SUM(H9:J9)</f>
+        <f t="shared" si="1"/>
         <v>0.17618819011041767</v>
       </c>
       <c r="P9">
-        <f>H9+I9</f>
+        <f t="shared" si="2"/>
         <v>1716</v>
       </c>
       <c r="R9">
@@ -5216,11 +5426,11 @@
         <v>1.2346715502656165</v>
       </c>
       <c r="Z9">
-        <f>U9/SUM(S9:U9)</f>
+        <f t="shared" si="3"/>
         <v>0.17618819011041767</v>
       </c>
       <c r="AA9">
-        <f>S9+T9</f>
+        <f t="shared" si="4"/>
         <v>17.16</v>
       </c>
     </row>
@@ -5238,35 +5448,35 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieNonIrrigatedNonFertilised</v>
       </c>
       <c r="F10" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>33491</v>
       </c>
       <c r="G10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3025</v>
       </c>
       <c r="H10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1873.9999999999998</v>
       </c>
       <c r="I10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>366</v>
       </c>
       <c r="J10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>532</v>
       </c>
       <c r="K10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>252.99999999999997</v>
       </c>
       <c r="L10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2772</v>
       </c>
       <c r="M10">
@@ -5276,11 +5486,11 @@
         <v>1.5272434546987774</v>
       </c>
       <c r="O10">
-        <f>J10/SUM(H10:J10)</f>
+        <f t="shared" si="1"/>
         <v>0.19191919191919191</v>
       </c>
       <c r="P10">
-        <f>H10+I10</f>
+        <f t="shared" si="2"/>
         <v>2240</v>
       </c>
       <c r="R10">
@@ -5308,11 +5518,11 @@
         <v>1.5272434546987774</v>
       </c>
       <c r="Z10">
-        <f>U10/SUM(S10:U10)</f>
+        <f t="shared" si="3"/>
         <v>0.19191919191919193</v>
       </c>
       <c r="AA10">
-        <f>S10+T10</f>
+        <f t="shared" si="4"/>
         <v>22.4</v>
       </c>
     </row>
@@ -5330,35 +5540,35 @@
         <v>5.6</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieNonIrrigatedNonFertilised</v>
       </c>
       <c r="F11" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>33856</v>
       </c>
       <c r="G11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4188</v>
       </c>
       <c r="H11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2590</v>
       </c>
       <c r="I11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>469.00000000000006</v>
       </c>
       <c r="J11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>815</v>
       </c>
       <c r="K11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>314</v>
       </c>
       <c r="L11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3874</v>
       </c>
       <c r="M11">
@@ -5368,11 +5578,11 @@
         <v>1.8928611151512691</v>
       </c>
       <c r="O11">
-        <f>J11/SUM(H11:J11)</f>
+        <f t="shared" si="1"/>
         <v>0.21037687145069695</v>
       </c>
       <c r="P11">
-        <f>H11+I11</f>
+        <f t="shared" si="2"/>
         <v>3059</v>
       </c>
       <c r="R11">
@@ -5400,11 +5610,11 @@
         <v>1.8928611151512691</v>
       </c>
       <c r="Z11">
-        <f>U11/SUM(S11:U11)</f>
+        <f t="shared" si="3"/>
         <v>0.21037687145069695</v>
       </c>
       <c r="AA11">
-        <f>S11+T11</f>
+        <f t="shared" si="4"/>
         <v>30.59</v>
       </c>
     </row>
@@ -5422,35 +5632,35 @@
         <v>0.66</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieIrrigatedNonFertilised</v>
       </c>
       <c r="F12" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32052.9</v>
       </c>
       <c r="G12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
       <c r="H12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="I12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="J12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="K12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="L12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>17</v>
       </c>
       <c r="M12">
@@ -5460,11 +5670,11 @@
         <v>0.16</v>
       </c>
       <c r="O12">
-        <f>J12/SUM(H12:J12)</f>
+        <f t="shared" si="1"/>
         <v>0.58823529411764708</v>
       </c>
       <c r="P12">
-        <f>H12+I12</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="R12">
@@ -5492,11 +5702,11 @@
         <v>0.16</v>
       </c>
       <c r="Z12">
-        <f>U12/SUM(S12:U12)</f>
+        <f t="shared" si="3"/>
         <v>0.58823529411764708</v>
       </c>
       <c r="AA12">
-        <f>S12+T12</f>
+        <f t="shared" si="4"/>
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
@@ -5514,35 +5724,35 @@
         <v>1.04</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieIrrigatedNonFertilised</v>
       </c>
       <c r="F13" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32191.599999999999</v>
       </c>
       <c r="G13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>438.99999999999994</v>
       </c>
       <c r="H13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>75</v>
       </c>
       <c r="I13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="J13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>168</v>
       </c>
       <c r="K13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>178</v>
       </c>
       <c r="L13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>261</v>
       </c>
       <c r="M13">
@@ -5552,11 +5762,11 @@
         <v>0.67</v>
       </c>
       <c r="O13">
-        <f>J13/SUM(H13:J13)</f>
+        <f t="shared" si="1"/>
         <v>0.64367816091954022</v>
       </c>
       <c r="P13">
-        <f>H13+I13</f>
+        <f t="shared" si="2"/>
         <v>93</v>
       </c>
       <c r="R13">
@@ -5584,11 +5794,11 @@
         <v>0.67</v>
       </c>
       <c r="Z13">
-        <f>U13/SUM(S13:U13)</f>
+        <f t="shared" si="3"/>
         <v>0.64367816091954022</v>
       </c>
       <c r="AA13">
-        <f>S13+T13</f>
+        <f t="shared" si="4"/>
         <v>0.92999999999999994</v>
       </c>
     </row>
@@ -5606,35 +5816,35 @@
         <v>1.44</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieIrrigatedNonFertilised</v>
       </c>
       <c r="F14" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32337.599999999999</v>
       </c>
       <c r="G14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>438.99999999999994</v>
       </c>
       <c r="H14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>123</v>
       </c>
       <c r="I14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>34</v>
       </c>
       <c r="J14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>140</v>
       </c>
       <c r="K14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>142</v>
       </c>
       <c r="L14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>297</v>
       </c>
       <c r="M14">
@@ -5644,11 +5854,11 @@
         <v>1.37</v>
       </c>
       <c r="O14">
-        <f>J14/SUM(H14:J14)</f>
+        <f t="shared" si="1"/>
         <v>0.4713804713804714</v>
       </c>
       <c r="P14">
-        <f>H14+I14</f>
+        <f t="shared" si="2"/>
         <v>157</v>
       </c>
       <c r="R14">
@@ -5676,11 +5886,11 @@
         <v>1.37</v>
       </c>
       <c r="Z14">
-        <f>U14/SUM(S14:U14)</f>
+        <f t="shared" si="3"/>
         <v>0.4713804713804714</v>
       </c>
       <c r="AA14">
-        <f>S14+T14</f>
+        <f t="shared" si="4"/>
         <v>1.57</v>
       </c>
     </row>
@@ -5698,35 +5908,35 @@
         <v>1.81</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieIrrigatedNonFertilised</v>
       </c>
       <c r="F15" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32472.65</v>
       </c>
       <c r="G15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>501</v>
       </c>
       <c r="H15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>249.00000000000003</v>
       </c>
       <c r="I15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>62</v>
       </c>
       <c r="J15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>90</v>
       </c>
       <c r="K15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>100</v>
       </c>
       <c r="L15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>401</v>
       </c>
       <c r="M15">
@@ -5736,11 +5946,11 @@
         <v>1.02</v>
       </c>
       <c r="O15">
-        <f>J15/SUM(H15:J15)</f>
+        <f t="shared" si="1"/>
         <v>0.22443890274314215</v>
       </c>
       <c r="P15">
-        <f>H15+I15</f>
+        <f t="shared" si="2"/>
         <v>311</v>
       </c>
       <c r="R15">
@@ -5768,11 +5978,11 @@
         <v>1.02</v>
       </c>
       <c r="Z15">
-        <f>U15/SUM(S15:U15)</f>
+        <f t="shared" si="3"/>
         <v>0.2244389027431421</v>
       </c>
       <c r="AA15">
-        <f>S15+T15</f>
+        <f t="shared" si="4"/>
         <v>3.1100000000000003</v>
       </c>
     </row>
@@ -5790,35 +6000,35 @@
         <v>2.4</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieIrrigatedNonFertilised</v>
       </c>
       <c r="F16" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32688</v>
       </c>
       <c r="G16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>713</v>
       </c>
       <c r="H16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>397</v>
       </c>
       <c r="I16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>94</v>
       </c>
       <c r="J16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>107</v>
       </c>
       <c r="K16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>114.99999999999999</v>
       </c>
       <c r="L16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>598</v>
       </c>
       <c r="M16">
@@ -5828,11 +6038,11 @@
         <v>1.17</v>
       </c>
       <c r="O16">
-        <f>J16/SUM(H16:J16)</f>
+        <f t="shared" si="1"/>
         <v>0.17892976588628762</v>
       </c>
       <c r="P16">
-        <f>H16+I16</f>
+        <f t="shared" si="2"/>
         <v>491</v>
       </c>
       <c r="R16">
@@ -5860,11 +6070,11 @@
         <v>1.17</v>
       </c>
       <c r="Z16">
-        <f>U16/SUM(S16:U16)</f>
+        <f t="shared" si="3"/>
         <v>0.17892976588628762</v>
       </c>
       <c r="AA16">
-        <f>S16+T16</f>
+        <f t="shared" si="4"/>
         <v>4.91</v>
       </c>
     </row>
@@ -5882,35 +6092,35 @@
         <v>3.1</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieIrrigatedNonFertilised</v>
       </c>
       <c r="F17" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32943.5</v>
       </c>
       <c r="G17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1257</v>
       </c>
       <c r="H17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>794</v>
       </c>
       <c r="I17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>183</v>
       </c>
       <c r="J17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>146</v>
       </c>
       <c r="K17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>134</v>
       </c>
       <c r="L17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1123</v>
       </c>
       <c r="M17">
@@ -5920,11 +6130,11 @@
         <v>0.8641386971188576</v>
       </c>
       <c r="O17">
-        <f>J17/SUM(H17:J17)</f>
+        <f t="shared" si="1"/>
         <v>0.13000890471950133</v>
       </c>
       <c r="P17">
-        <f>H17+I17</f>
+        <f t="shared" si="2"/>
         <v>977</v>
       </c>
       <c r="R17">
@@ -5952,11 +6162,11 @@
         <v>0.8641386971188576</v>
       </c>
       <c r="Z17">
-        <f>U17/SUM(S17:U17)</f>
+        <f t="shared" si="3"/>
         <v>0.13000890471950133</v>
       </c>
       <c r="AA17">
-        <f>S17+T17</f>
+        <f t="shared" si="4"/>
         <v>9.77</v>
       </c>
     </row>
@@ -5974,35 +6184,35 @@
         <v>3.6</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieIrrigatedNonFertilised</v>
       </c>
       <c r="F18" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>33126</v>
       </c>
       <c r="G18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1544</v>
       </c>
       <c r="H18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>957</v>
       </c>
       <c r="I18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>219</v>
       </c>
       <c r="J18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>216</v>
       </c>
       <c r="K18">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>152</v>
       </c>
       <c r="L18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1392</v>
       </c>
       <c r="M18">
@@ -6012,11 +6222,11 @@
         <v>0.9262639277357525</v>
       </c>
       <c r="O18">
-        <f>J18/SUM(H18:J18)</f>
+        <f t="shared" si="1"/>
         <v>0.15517241379310345</v>
       </c>
       <c r="P18">
-        <f>H18+I18</f>
+        <f t="shared" si="2"/>
         <v>1176</v>
       </c>
       <c r="R18">
@@ -6044,11 +6254,11 @@
         <v>0.9262639277357525</v>
       </c>
       <c r="Z18">
-        <f>U18/SUM(S18:U18)</f>
+        <f t="shared" si="3"/>
         <v>0.15517241379310345</v>
       </c>
       <c r="AA18">
-        <f>S18+T18</f>
+        <f t="shared" si="4"/>
         <v>11.76</v>
       </c>
     </row>
@@ -6066,35 +6276,35 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieIrrigatedNonFertilised</v>
       </c>
       <c r="F19" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>33308.5</v>
       </c>
       <c r="G19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1960.0000000000002</v>
       </c>
       <c r="H19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1199</v>
       </c>
       <c r="I19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>267</v>
       </c>
       <c r="J19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>314</v>
       </c>
       <c r="K19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>180</v>
       </c>
       <c r="L19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1780</v>
       </c>
       <c r="M19">
@@ -6104,11 +6314,11 @@
         <v>1.091920584234471</v>
       </c>
       <c r="O19">
-        <f>J19/SUM(H19:J19)</f>
+        <f t="shared" si="1"/>
         <v>0.17640449438202246</v>
       </c>
       <c r="P19">
-        <f>H19+I19</f>
+        <f t="shared" si="2"/>
         <v>1466</v>
       </c>
       <c r="R19">
@@ -6136,11 +6346,11 @@
         <v>1.091920584234471</v>
       </c>
       <c r="Z19">
-        <f>U19/SUM(S19:U19)</f>
+        <f t="shared" si="3"/>
         <v>0.17640449438202246</v>
       </c>
       <c r="AA19">
-        <f>S19+T19</f>
+        <f t="shared" si="4"/>
         <v>14.66</v>
       </c>
     </row>
@@ -6158,35 +6368,35 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieIrrigatedNonFertilised</v>
       </c>
       <c r="F20" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>33491</v>
       </c>
       <c r="G20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2785</v>
       </c>
       <c r="H20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1692.0000000000002</v>
       </c>
       <c r="I20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>355</v>
       </c>
       <c r="J20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>499</v>
       </c>
       <c r="K20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>239</v>
       </c>
       <c r="L20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2546</v>
       </c>
       <c r="M20">
@@ -6196,11 +6406,11 @@
         <v>1.4467260957771373</v>
       </c>
       <c r="O20">
-        <f>J20/SUM(H20:J20)</f>
+        <f t="shared" si="1"/>
         <v>0.19599371563236451</v>
       </c>
       <c r="P20">
-        <f>H20+I20</f>
+        <f t="shared" si="2"/>
         <v>2047.0000000000002</v>
       </c>
       <c r="R20">
@@ -6228,11 +6438,11 @@
         <v>1.4467260957771373</v>
       </c>
       <c r="Z20">
-        <f>U20/SUM(S20:U20)</f>
+        <f t="shared" si="3"/>
         <v>0.19599371563236451</v>
       </c>
       <c r="AA20">
-        <f>S20+T20</f>
+        <f t="shared" si="4"/>
         <v>20.470000000000002</v>
       </c>
     </row>
@@ -6250,35 +6460,35 @@
         <v>5.6</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieIrrigatedNonFertilised</v>
       </c>
       <c r="F21" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>33856</v>
       </c>
       <c r="G21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4184</v>
       </c>
       <c r="H21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2540</v>
       </c>
       <c r="I21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>484.99999999999994</v>
       </c>
       <c r="J21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>836.99999999999989</v>
       </c>
       <c r="K21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>322</v>
       </c>
       <c r="L21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3861.9999999999995</v>
       </c>
       <c r="M21">
@@ -6288,11 +6498,11 @@
         <v>1.9418855403379214</v>
       </c>
       <c r="O21">
-        <f>J21/SUM(H21:J21)</f>
+        <f t="shared" si="1"/>
         <v>0.2167270844122216</v>
       </c>
       <c r="P21">
-        <f>H21+I21</f>
+        <f t="shared" si="2"/>
         <v>3025</v>
       </c>
       <c r="R21">
@@ -6320,11 +6530,11 @@
         <v>1.9418855403379214</v>
       </c>
       <c r="Z21">
-        <f>U21/SUM(S21:U21)</f>
+        <f t="shared" si="3"/>
         <v>0.21672708441222163</v>
       </c>
       <c r="AA21">
-        <f>S21+T21</f>
+        <f t="shared" si="4"/>
         <v>30.25</v>
       </c>
     </row>
@@ -6342,35 +6552,35 @@
         <v>0.66</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieNonIrrigatedFertilised</v>
       </c>
       <c r="F22" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32052.9</v>
       </c>
       <c r="G22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>508</v>
       </c>
       <c r="H22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>86</v>
       </c>
       <c r="I22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>21</v>
       </c>
       <c r="J22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>194</v>
       </c>
       <c r="K22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>206.99999999999997</v>
       </c>
       <c r="L22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>301</v>
       </c>
       <c r="M22">
@@ -6380,11 +6590,11 @@
         <v>1.82</v>
       </c>
       <c r="O22">
-        <f>J22/SUM(H22:J22)</f>
+        <f t="shared" si="1"/>
         <v>0.64451827242524917</v>
       </c>
       <c r="P22">
-        <f>H22+I22</f>
+        <f t="shared" si="2"/>
         <v>107</v>
       </c>
       <c r="R22">
@@ -6412,11 +6622,11 @@
         <v>1.82</v>
       </c>
       <c r="Z22">
-        <f>U22/SUM(S22:U22)</f>
+        <f t="shared" si="3"/>
         <v>0.64451827242524917</v>
       </c>
       <c r="AA22">
-        <f>S22+T22</f>
+        <f t="shared" si="4"/>
         <v>1.07</v>
       </c>
     </row>
@@ -6434,35 +6644,35 @@
         <v>1.04</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieNonIrrigatedFertilised</v>
       </c>
       <c r="F23" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32191.599999999999</v>
       </c>
       <c r="G23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1687</v>
       </c>
       <c r="H23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>562</v>
       </c>
       <c r="I23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>117</v>
       </c>
       <c r="J23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>584</v>
       </c>
       <c r="K23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>425</v>
       </c>
       <c r="L23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1262</v>
       </c>
       <c r="M23">
@@ -6472,11 +6682,11 @@
         <v>4.46</v>
       </c>
       <c r="O23">
-        <f>J23/SUM(H23:J23)</f>
+        <f t="shared" si="1"/>
         <v>0.46239113222486145</v>
       </c>
       <c r="P23">
-        <f>H23+I23</f>
+        <f t="shared" si="2"/>
         <v>679</v>
       </c>
       <c r="R23">
@@ -6504,11 +6714,11 @@
         <v>4.46</v>
       </c>
       <c r="Z23">
-        <f>U23/SUM(S23:U23)</f>
+        <f t="shared" si="3"/>
         <v>0.46239113222486145</v>
       </c>
       <c r="AA23">
-        <f>S23+T23</f>
+        <f t="shared" si="4"/>
         <v>6.79</v>
       </c>
     </row>
@@ -6526,35 +6736,35 @@
         <v>1.44</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieNonIrrigatedFertilised</v>
       </c>
       <c r="F24" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32337.599999999999</v>
       </c>
       <c r="G24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2581</v>
       </c>
       <c r="H24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1146</v>
       </c>
       <c r="I24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>213</v>
       </c>
       <c r="J24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>730</v>
       </c>
       <c r="K24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>492</v>
       </c>
       <c r="L24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2089</v>
       </c>
       <c r="M24">
@@ -6564,11 +6774,11 @@
         <v>4.8099999999999996</v>
       </c>
       <c r="O24">
-        <f>J24/SUM(H24:J24)</f>
+        <f t="shared" si="1"/>
         <v>0.3494494973671613</v>
       </c>
       <c r="P24">
-        <f>H24+I24</f>
+        <f t="shared" si="2"/>
         <v>1359</v>
       </c>
       <c r="R24">
@@ -6596,11 +6806,11 @@
         <v>4.8099999999999996</v>
       </c>
       <c r="Z24">
-        <f>U24/SUM(S24:U24)</f>
+        <f t="shared" si="3"/>
         <v>0.3494494973671613</v>
       </c>
       <c r="AA24">
-        <f>S24+T24</f>
+        <f t="shared" si="4"/>
         <v>13.59</v>
       </c>
     </row>
@@ -6618,35 +6828,35 @@
         <v>1.81</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieNonIrrigatedFertilised</v>
       </c>
       <c r="F25" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32472.65</v>
       </c>
       <c r="G25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3347</v>
       </c>
       <c r="H25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1918</v>
       </c>
       <c r="I25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>330</v>
       </c>
       <c r="J25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>643</v>
       </c>
       <c r="K25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>455.99999999999994</v>
       </c>
       <c r="L25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2891</v>
       </c>
       <c r="M25">
@@ -6656,11 +6866,11 @@
         <v>4.79</v>
       </c>
       <c r="O25">
-        <f>J25/SUM(H25:J25)</f>
+        <f t="shared" si="1"/>
         <v>0.2224143894846074</v>
       </c>
       <c r="P25">
-        <f>H25+I25</f>
+        <f t="shared" si="2"/>
         <v>2248</v>
       </c>
       <c r="R25">
@@ -6688,11 +6898,11 @@
         <v>4.79</v>
       </c>
       <c r="Z25">
-        <f>U25/SUM(S25:U25)</f>
+        <f t="shared" si="3"/>
         <v>0.2224143894846074</v>
       </c>
       <c r="AA25">
-        <f>S25+T25</f>
+        <f t="shared" si="4"/>
         <v>22.48</v>
       </c>
     </row>
@@ -6710,35 +6920,35 @@
         <v>2.4</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieNonIrrigatedFertilised</v>
       </c>
       <c r="F26" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32688</v>
       </c>
       <c r="G26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4990</v>
       </c>
       <c r="H26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3201</v>
       </c>
       <c r="I26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>509.99999999999994</v>
       </c>
       <c r="J26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>762</v>
       </c>
       <c r="K26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>516</v>
       </c>
       <c r="L26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4474</v>
       </c>
       <c r="M26">
@@ -6748,11 +6958,11 @@
         <v>5.17</v>
       </c>
       <c r="O26">
-        <f>J26/SUM(H26:J26)</f>
+        <f t="shared" si="1"/>
         <v>0.17035546613011401</v>
       </c>
       <c r="P26">
-        <f>H26+I26</f>
+        <f t="shared" si="2"/>
         <v>3711</v>
       </c>
       <c r="R26">
@@ -6780,11 +6990,11 @@
         <v>5.17</v>
       </c>
       <c r="Z26">
-        <f>U26/SUM(S26:U26)</f>
+        <f t="shared" si="3"/>
         <v>0.17035546613011404</v>
       </c>
       <c r="AA26">
-        <f>S26+T26</f>
+        <f t="shared" si="4"/>
         <v>37.11</v>
       </c>
     </row>
@@ -6802,35 +7012,35 @@
         <v>3.1</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieNonIrrigatedFertilised</v>
       </c>
       <c r="F27" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32943.5</v>
       </c>
       <c r="G27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>7203</v>
       </c>
       <c r="H27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4543</v>
       </c>
       <c r="I27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>727</v>
       </c>
       <c r="J27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1223</v>
       </c>
       <c r="K27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>710</v>
       </c>
       <c r="L27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>6493.0000000000009</v>
       </c>
       <c r="M27">
@@ -6840,11 +7050,11 @@
         <v>4.3050987125831597</v>
       </c>
       <c r="O27">
-        <f>J27/SUM(H27:J27)</f>
+        <f t="shared" si="1"/>
         <v>0.1883566918219621</v>
       </c>
       <c r="P27">
-        <f>H27+I27</f>
+        <f t="shared" si="2"/>
         <v>5270</v>
       </c>
       <c r="R27">
@@ -6872,11 +7082,11 @@
         <v>4.3050987125831597</v>
       </c>
       <c r="Z27">
-        <f>U27/SUM(S27:U27)</f>
+        <f t="shared" si="3"/>
         <v>0.1883566918219621</v>
       </c>
       <c r="AA27">
-        <f>S27+T27</f>
+        <f t="shared" si="4"/>
         <v>52.7</v>
       </c>
     </row>
@@ -6894,35 +7104,35 @@
         <v>3.6</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieNonIrrigatedFertilised</v>
       </c>
       <c r="F28" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>33126</v>
       </c>
       <c r="G28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>8305</v>
       </c>
       <c r="H28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5250</v>
       </c>
       <c r="I28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>838.00000000000011</v>
       </c>
       <c r="J28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1460</v>
       </c>
       <c r="K28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>757</v>
       </c>
       <c r="L28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>7548</v>
       </c>
       <c r="M28">
@@ -6932,11 +7142,11 @@
         <v>4.5350863800777814</v>
       </c>
       <c r="O28">
-        <f>J28/SUM(H28:J28)</f>
+        <f t="shared" si="1"/>
         <v>0.19342872284048754</v>
       </c>
       <c r="P28">
-        <f>H28+I28</f>
+        <f t="shared" si="2"/>
         <v>6088</v>
       </c>
       <c r="R28">
@@ -6964,11 +7174,11 @@
         <v>4.5350863800777814</v>
       </c>
       <c r="Z28">
-        <f>U28/SUM(S28:U28)</f>
+        <f t="shared" si="3"/>
         <v>0.19342872284048754</v>
       </c>
       <c r="AA28">
-        <f>S28+T28</f>
+        <f t="shared" si="4"/>
         <v>60.88</v>
       </c>
     </row>
@@ -6986,35 +7196,35 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieNonIrrigatedFertilised</v>
       </c>
       <c r="F29" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>33308.5</v>
       </c>
       <c r="G29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>9295</v>
       </c>
       <c r="H29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5883</v>
       </c>
       <c r="I29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>935</v>
       </c>
       <c r="J29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1686</v>
       </c>
       <c r="K29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>791</v>
       </c>
       <c r="L29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>8504</v>
       </c>
       <c r="M29">
@@ -7024,11 +7234,11 @@
         <v>4.7366539061573079</v>
       </c>
       <c r="O29">
-        <f>J29/SUM(H29:J29)</f>
+        <f t="shared" si="1"/>
         <v>0.19825964252116651</v>
       </c>
       <c r="P29">
-        <f>H29+I29</f>
+        <f t="shared" si="2"/>
         <v>6818</v>
       </c>
       <c r="R29">
@@ -7056,11 +7266,11 @@
         <v>4.7366539061573079</v>
       </c>
       <c r="Z29">
-        <f>U29/SUM(S29:U29)</f>
+        <f t="shared" si="3"/>
         <v>0.19825964252116651</v>
       </c>
       <c r="AA29">
-        <f>S29+T29</f>
+        <f t="shared" si="4"/>
         <v>68.179999999999993</v>
       </c>
     </row>
@@ -7078,35 +7288,35 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieNonIrrigatedFertilised</v>
       </c>
       <c r="F30" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>33491</v>
       </c>
       <c r="G30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>10620</v>
       </c>
       <c r="H30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>6776.0000000000009</v>
       </c>
       <c r="I30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1056</v>
       </c>
       <c r="J30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1989</v>
       </c>
       <c r="K30">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>851</v>
       </c>
       <c r="L30">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>9769</v>
       </c>
       <c r="M30">
@@ -7116,11 +7326,11 @@
         <v>5.0975221261983501</v>
       </c>
       <c r="O30">
-        <f>J30/SUM(H30:J30)</f>
+        <f t="shared" si="1"/>
         <v>0.20252520109968436</v>
       </c>
       <c r="P30">
-        <f>H30+I30</f>
+        <f t="shared" si="2"/>
         <v>7832.0000000000009</v>
       </c>
       <c r="R30">
@@ -7148,11 +7358,11 @@
         <v>5.0975221261983501</v>
       </c>
       <c r="Z30">
-        <f>U30/SUM(S30:U30)</f>
+        <f t="shared" si="3"/>
         <v>0.20252520109968433</v>
       </c>
       <c r="AA30">
-        <f>S30+T30</f>
+        <f t="shared" si="4"/>
         <v>78.320000000000007</v>
       </c>
     </row>
@@ -7170,35 +7380,35 @@
         <v>5.6</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieNonIrrigatedFertilised</v>
       </c>
       <c r="F31" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>33856</v>
       </c>
       <c r="G31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>13559</v>
       </c>
       <c r="H31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>8660</v>
       </c>
       <c r="I31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1270</v>
       </c>
       <c r="J31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2659</v>
       </c>
       <c r="K31">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>969.99999999999989</v>
       </c>
       <c r="L31">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>12589</v>
       </c>
       <c r="M31">
@@ -7208,11 +7418,11 @@
         <v>5.8077451577125405</v>
       </c>
       <c r="O31">
-        <f>J31/SUM(H31:J31)</f>
+        <f t="shared" si="1"/>
         <v>0.21121614107554215</v>
       </c>
       <c r="P31">
-        <f>H31+I31</f>
+        <f t="shared" si="2"/>
         <v>9930</v>
       </c>
       <c r="R31">
@@ -7240,11 +7450,11 @@
         <v>5.8077451577125405</v>
       </c>
       <c r="Z31">
-        <f>U31/SUM(S31:U31)</f>
+        <f t="shared" si="3"/>
         <v>0.21121614107554212</v>
       </c>
       <c r="AA31">
-        <f>S31+T31</f>
+        <f t="shared" si="4"/>
         <v>99.3</v>
       </c>
     </row>
@@ -7262,35 +7472,35 @@
         <v>0.66</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieIrrigatedFertilised</v>
       </c>
       <c r="F32" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32052.9</v>
       </c>
       <c r="G32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>609</v>
       </c>
       <c r="H32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>104</v>
       </c>
       <c r="I32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>24</v>
       </c>
       <c r="J32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>237</v>
       </c>
       <c r="K32">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>243.00000000000003</v>
       </c>
       <c r="L32">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>366</v>
       </c>
       <c r="M32">
@@ -7300,11 +7510,11 @@
         <v>2.0099999999999998</v>
       </c>
       <c r="O32">
-        <f>J32/SUM(H32:J32)</f>
+        <f t="shared" si="1"/>
         <v>0.64931506849315068</v>
       </c>
       <c r="P32">
-        <f>H32+I32</f>
+        <f t="shared" si="2"/>
         <v>128</v>
       </c>
       <c r="R32">
@@ -7332,11 +7542,11 @@
         <v>2.0099999999999998</v>
       </c>
       <c r="Z32">
-        <f>U32/SUM(S32:U32)</f>
+        <f t="shared" si="3"/>
         <v>0.64931506849315068</v>
       </c>
       <c r="AA32">
-        <f>S32+T32</f>
+        <f t="shared" si="4"/>
         <v>1.28</v>
       </c>
     </row>
@@ -7354,35 +7564,35 @@
         <v>1.04</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieIrrigatedFertilised</v>
       </c>
       <c r="F33" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32191.599999999999</v>
       </c>
       <c r="G33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1944.0000000000002</v>
       </c>
       <c r="H33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>685</v>
       </c>
       <c r="I33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>135</v>
       </c>
       <c r="J33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>660</v>
       </c>
       <c r="K33">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>465.00000000000006</v>
       </c>
       <c r="L33">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1479</v>
       </c>
       <c r="M33">
@@ -7392,11 +7602,11 @@
         <v>4.95</v>
       </c>
       <c r="O33">
-        <f>J33/SUM(H33:J33)</f>
+        <f t="shared" si="1"/>
         <v>0.44594594594594594</v>
       </c>
       <c r="P33">
-        <f>H33+I33</f>
+        <f t="shared" si="2"/>
         <v>820</v>
       </c>
       <c r="R33">
@@ -7424,11 +7634,11 @@
         <v>4.95</v>
       </c>
       <c r="Z33">
-        <f>U33/SUM(S33:U33)</f>
+        <f t="shared" si="3"/>
         <v>0.44594594594594594</v>
       </c>
       <c r="AA33">
-        <f>S33+T33</f>
+        <f t="shared" si="4"/>
         <v>8.1999999999999993</v>
       </c>
     </row>
@@ -7446,35 +7656,35 @@
         <v>1.44</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieIrrigatedFertilised</v>
       </c>
       <c r="F34" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32337.599999999999</v>
       </c>
       <c r="G34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2437</v>
       </c>
       <c r="H34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1055</v>
       </c>
       <c r="I34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>189</v>
       </c>
       <c r="J34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>725</v>
       </c>
       <c r="K34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>468</v>
       </c>
       <c r="L34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1969.0000000000002</v>
       </c>
       <c r="M34">
@@ -7484,11 +7694,11 @@
         <v>4.5</v>
       </c>
       <c r="O34">
-        <f>J34/SUM(H34:J34)</f>
+        <f t="shared" si="1"/>
         <v>0.36820721178263077</v>
       </c>
       <c r="P34">
-        <f>H34+I34</f>
+        <f t="shared" si="2"/>
         <v>1244</v>
       </c>
       <c r="R34">
@@ -7516,11 +7726,11 @@
         <v>4.5</v>
       </c>
       <c r="Z34">
-        <f>U34/SUM(S34:U34)</f>
+        <f t="shared" si="3"/>
         <v>0.36820721178263077</v>
       </c>
       <c r="AA34">
-        <f>S34+T34</f>
+        <f t="shared" si="4"/>
         <v>12.440000000000001</v>
       </c>
     </row>
@@ -7538,35 +7748,35 @@
         <v>1.81</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieIrrigatedFertilised</v>
       </c>
       <c r="F35" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32472.65</v>
       </c>
       <c r="G35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3062</v>
       </c>
       <c r="H35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>1596</v>
       </c>
       <c r="I35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>264</v>
       </c>
       <c r="J35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>741</v>
       </c>
       <c r="K35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>459.99999999999994</v>
       </c>
       <c r="L35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2602</v>
       </c>
       <c r="M35">
@@ -7576,11 +7786,11 @@
         <v>4.29</v>
       </c>
       <c r="O35">
-        <f>J35/SUM(H35:J35)</f>
+        <f t="shared" si="1"/>
         <v>0.28489042675893889</v>
       </c>
       <c r="P35">
-        <f>H35+I35</f>
+        <f t="shared" si="2"/>
         <v>1860</v>
       </c>
       <c r="R35">
@@ -7608,11 +7818,11 @@
         <v>4.29</v>
       </c>
       <c r="Z35">
-        <f>U35/SUM(S35:U35)</f>
+        <f t="shared" si="3"/>
         <v>0.28489042675893883</v>
       </c>
       <c r="AA35">
-        <f>S35+T35</f>
+        <f t="shared" si="4"/>
         <v>18.600000000000001</v>
       </c>
     </row>
@@ -7630,35 +7840,35 @@
         <v>2.4</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieIrrigatedFertilised</v>
       </c>
       <c r="F36" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32688</v>
       </c>
       <c r="G36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>3888.0000000000005</v>
       </c>
       <c r="H36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>2491</v>
       </c>
       <c r="I36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>384</v>
       </c>
       <c r="J36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>617</v>
       </c>
       <c r="K36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>396</v>
       </c>
       <c r="L36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3492</v>
       </c>
       <c r="M36">
@@ -7668,11 +7878,11 @@
         <v>3.87</v>
       </c>
       <c r="O36">
-        <f>J36/SUM(H36:J36)</f>
+        <f t="shared" si="1"/>
         <v>0.17668957617411227</v>
       </c>
       <c r="P36">
-        <f>H36+I36</f>
+        <f t="shared" si="2"/>
         <v>2875</v>
       </c>
       <c r="R36">
@@ -7700,11 +7910,11 @@
         <v>3.87</v>
       </c>
       <c r="Z36">
-        <f>U36/SUM(S36:U36)</f>
+        <f t="shared" si="3"/>
         <v>0.17668957617411224</v>
       </c>
       <c r="AA36">
-        <f>S36+T36</f>
+        <f t="shared" si="4"/>
         <v>28.75</v>
       </c>
     </row>
@@ -7722,35 +7932,35 @@
         <v>3.1</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieIrrigatedFertilised</v>
       </c>
       <c r="F37" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>32943.5</v>
       </c>
       <c r="G37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>6311</v>
       </c>
       <c r="H37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4047.9999999999995</v>
       </c>
       <c r="I37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>609</v>
       </c>
       <c r="J37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1018</v>
       </c>
       <c r="K37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>600</v>
       </c>
       <c r="L37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>5711</v>
       </c>
       <c r="M37">
@@ -7760,11 +7970,11 @@
         <v>3.6865749439928703</v>
       </c>
       <c r="O37">
-        <f>J37/SUM(H37:J37)</f>
+        <f t="shared" si="1"/>
         <v>0.17938325991189427</v>
       </c>
       <c r="P37">
-        <f>H37+I37</f>
+        <f t="shared" si="2"/>
         <v>4657</v>
       </c>
       <c r="R37">
@@ -7792,11 +8002,11 @@
         <v>3.6865749439928703</v>
       </c>
       <c r="Z37">
-        <f>U37/SUM(S37:U37)</f>
+        <f t="shared" si="3"/>
         <v>0.1793832599118943</v>
       </c>
       <c r="AA37">
-        <f>S37+T37</f>
+        <f t="shared" si="4"/>
         <v>46.569999999999993</v>
       </c>
     </row>
@@ -7814,35 +8024,35 @@
         <v>3.6</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieIrrigatedFertilised</v>
       </c>
       <c r="F38" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>33126</v>
       </c>
       <c r="G38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>7158</v>
       </c>
       <c r="H38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4632</v>
       </c>
       <c r="I38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>694</v>
       </c>
       <c r="J38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1201</v>
       </c>
       <c r="K38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>631</v>
       </c>
       <c r="L38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>6527</v>
       </c>
       <c r="M38">
@@ -7852,11 +8062,11 @@
         <v>3.7855418070094617</v>
       </c>
       <c r="O38">
-        <f>J38/SUM(H38:J38)</f>
+        <f t="shared" si="1"/>
         <v>0.18400490271181247</v>
       </c>
       <c r="P38">
-        <f>H38+I38</f>
+        <f t="shared" si="2"/>
         <v>5326</v>
       </c>
       <c r="R38">
@@ -7884,11 +8094,11 @@
         <v>3.7855418070094617</v>
       </c>
       <c r="Z38">
-        <f>U38/SUM(S38:U38)</f>
+        <f t="shared" si="3"/>
         <v>0.18400490271181247</v>
       </c>
       <c r="AA38">
-        <f>S38+T38</f>
+        <f t="shared" si="4"/>
         <v>53.26</v>
       </c>
     </row>
@@ -7906,35 +8116,35 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieIrrigatedFertilised</v>
       </c>
       <c r="F39" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>33308.5</v>
       </c>
       <c r="G39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>8083</v>
       </c>
       <c r="H39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>5233</v>
       </c>
       <c r="I39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>781</v>
       </c>
       <c r="J39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1404</v>
       </c>
       <c r="K39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>665</v>
       </c>
       <c r="L39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>7418.0000000000009</v>
       </c>
       <c r="M39">
@@ -7944,11 +8154,11 @@
         <v>3.9889772338145639</v>
       </c>
       <c r="O39">
-        <f>J39/SUM(H39:J39)</f>
+        <f t="shared" si="1"/>
         <v>0.18926934483688326</v>
       </c>
       <c r="P39">
-        <f>H39+I39</f>
+        <f t="shared" si="2"/>
         <v>6014</v>
       </c>
       <c r="R39">
@@ -7976,11 +8186,11 @@
         <v>3.9889772338145639</v>
       </c>
       <c r="Z39">
-        <f>U39/SUM(S39:U39)</f>
+        <f t="shared" si="3"/>
         <v>0.18926934483688324</v>
       </c>
       <c r="AA39">
-        <f>S39+T39</f>
+        <f t="shared" si="4"/>
         <v>60.14</v>
       </c>
     </row>
@@ -7998,35 +8208,35 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieIrrigatedFertilised</v>
       </c>
       <c r="F40" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>33491</v>
       </c>
       <c r="G40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>9853</v>
       </c>
       <c r="H40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>6409.9999999999991</v>
       </c>
       <c r="I40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>926</v>
       </c>
       <c r="J40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1760.0000000000002</v>
       </c>
       <c r="K40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>757</v>
       </c>
       <c r="L40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>9096</v>
       </c>
       <c r="M40">
@@ -8036,11 +8246,11 @@
         <v>4.5351055053411846</v>
       </c>
       <c r="O40">
-        <f>J40/SUM(H40:J40)</f>
+        <f t="shared" si="1"/>
         <v>0.19349164467897981</v>
       </c>
       <c r="P40">
-        <f>H40+I40</f>
+        <f t="shared" si="2"/>
         <v>7335.9999999999991</v>
       </c>
       <c r="R40">
@@ -8068,11 +8278,11 @@
         <v>4.5351055053411846</v>
       </c>
       <c r="Z40">
-        <f>U40/SUM(S40:U40)</f>
+        <f t="shared" si="3"/>
         <v>0.19349164467897978</v>
       </c>
       <c r="AA40">
-        <f>S40+T40</f>
+        <f t="shared" si="4"/>
         <v>73.36</v>
       </c>
     </row>
@@ -8090,35 +8300,35 @@
         <v>5.6</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>GympieIrrigatedFertilised</v>
       </c>
       <c r="F41" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>33856</v>
       </c>
       <c r="G41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>13702.000000000002</v>
       </c>
       <c r="H41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>9000</v>
       </c>
       <c r="I41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1199</v>
       </c>
       <c r="J41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2566</v>
       </c>
       <c r="K41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>936.99999999999989</v>
       </c>
       <c r="L41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>12765</v>
       </c>
       <c r="M41">
@@ -8128,11 +8338,11 @@
         <v>5.3922041846935125</v>
       </c>
       <c r="O41">
-        <f>J41/SUM(H41:J41)</f>
+        <f t="shared" si="1"/>
         <v>0.20101840971406187</v>
       </c>
       <c r="P41">
-        <f>H41+I41</f>
+        <f t="shared" si="2"/>
         <v>10199</v>
       </c>
       <c r="R41">
@@ -8160,11 +8370,11 @@
         <v>5.3922041846935125</v>
       </c>
       <c r="Z41">
-        <f>U41/SUM(S41:U41)</f>
+        <f t="shared" si="3"/>
         <v>0.2010184097140619</v>
       </c>
       <c r="AA41">
-        <f>S41+T41</f>
+        <f t="shared" si="4"/>
         <v>101.99</v>
       </c>
     </row>
@@ -8177,7 +8387,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J97"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11128,10 +11338,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
@@ -11164,10 +11374,10 @@
         <v>2</v>
       </c>
       <c r="I1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -11184,7 +11394,7 @@
         <v>1E-3</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G2">
         <f>A2</f>
@@ -11217,7 +11427,7 @@
         <v>1E-3</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G48" si="0">A3</f>
@@ -11250,7 +11460,7 @@
         <v>1E-3</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
@@ -11283,7 +11493,7 @@
         <v>1E-3</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
@@ -11316,7 +11526,7 @@
         <v>1E-3</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
@@ -11349,7 +11559,7 @@
         <v>1E-3</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -11382,7 +11592,7 @@
         <v>1E-3</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
@@ -11415,7 +11625,7 @@
         <v>1E-3</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
@@ -11448,7 +11658,7 @@
         <v>1E-3</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
@@ -11481,7 +11691,7 @@
         <v>1E-3</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
@@ -11514,7 +11724,7 @@
         <v>1E-3</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
@@ -11547,7 +11757,7 @@
         <v>1E-3</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
@@ -11580,7 +11790,7 @@
         <v>1E-3</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
@@ -11613,7 +11823,7 @@
         <v>1E-3</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
@@ -11646,7 +11856,7 @@
         <v>1E-3</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
@@ -11679,7 +11889,7 @@
         <v>1E-3</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
@@ -11712,7 +11922,7 @@
         <v>1E-3</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
@@ -11745,7 +11955,7 @@
         <v>1E-3</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
@@ -11778,7 +11988,7 @@
         <v>1E-3</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
@@ -11811,7 +12021,7 @@
         <v>46.975000000000001</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
@@ -11844,7 +12054,7 @@
         <v>86.35</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G22">
         <f t="shared" si="0"/>
@@ -11877,7 +12087,7 @@
         <v>118.9</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
@@ -11910,7 +12120,7 @@
         <v>144.8125</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
@@ -11943,7 +12153,7 @@
         <v>192.0625</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G25">
         <f t="shared" si="0"/>
@@ -11976,7 +12186,7 @@
         <v>289.97500000000002</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
@@ -12009,7 +12219,7 @@
         <v>511.6</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
@@ -12042,7 +12252,7 @@
         <v>1128.05</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
@@ -12075,7 +12285,7 @@
         <v>2052.5749999999998</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G29">
         <f t="shared" si="0"/>
@@ -12108,7 +12318,7 @@
         <v>2985.5625</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G30">
         <f t="shared" si="0"/>
@@ -12141,7 +12351,7 @@
         <v>3708.4</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G31">
         <f t="shared" si="0"/>
@@ -12174,7 +12384,7 @@
         <v>4112.0625</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G32">
         <f t="shared" si="0"/>
@@ -12207,7 +12417,7 @@
         <v>4433.5874999999996</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G33">
         <f t="shared" si="0"/>
@@ -12240,7 +12450,7 @@
         <v>4645.8999999999996</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G34">
         <f t="shared" si="0"/>
@@ -12273,7 +12483,7 @@
         <v>4746.0749999999998</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G35">
         <f t="shared" si="0"/>
@@ -12306,7 +12516,7 @@
         <v>4809.6374999999998</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G36">
         <f t="shared" si="0"/>
@@ -12339,7 +12549,7 @@
         <v>4964.7249999999995</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G37">
         <f t="shared" si="0"/>
@@ -12372,7 +12582,7 @@
         <v>5184.3624999999993</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G38">
         <f t="shared" si="0"/>
@@ -12405,7 +12615,7 @@
         <v>5605.1124999999993</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G39">
         <f t="shared" si="0"/>
@@ -12438,7 +12648,7 @@
         <v>6265.3874999999989</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G40">
         <f t="shared" si="0"/>
@@ -12471,7 +12681,7 @@
         <v>7603.8249999999989</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G41">
         <f t="shared" si="0"/>
@@ -12504,7 +12714,7 @@
         <v>8152.2249999999985</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G42">
         <f t="shared" si="0"/>
@@ -12537,7 +12747,7 @@
         <v>8529.3874999999989</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G43">
         <f t="shared" si="0"/>
@@ -12570,7 +12780,7 @@
         <v>9184.4374999999982</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G44">
         <f t="shared" si="0"/>
@@ -12603,7 +12813,7 @@
         <v>9444.3624999999975</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G45">
         <f t="shared" si="0"/>
@@ -12636,7 +12846,7 @@
         <v>9649.2999999999993</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G46">
         <f t="shared" si="0"/>
@@ -12669,7 +12879,7 @@
         <v>9768.0374999999967</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G47">
         <f t="shared" si="0"/>
@@ -12702,7 +12912,7 @@
         <v>9820.6</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G48">
         <f t="shared" si="0"/>
@@ -12729,11 +12939,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -12774,13 +12984,13 @@
         <v>2</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M1" s="8" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -12808,7 +13018,7 @@
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J2" s="5">
         <f>B2</f>
@@ -12853,7 +13063,7 @@
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" ref="J3:J48" si="1">B3</f>
@@ -12898,7 +13108,7 @@
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J4" s="5">
         <f t="shared" si="1"/>
@@ -12943,7 +13153,7 @@
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" si="1"/>
@@ -12988,7 +13198,7 @@
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="1"/>
@@ -13033,7 +13243,7 @@
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="1"/>
@@ -13078,7 +13288,7 @@
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" si="1"/>
@@ -13123,7 +13333,7 @@
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="1"/>
@@ -13168,7 +13378,7 @@
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J10" s="5">
         <f t="shared" si="1"/>
@@ -13213,7 +13423,7 @@
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" si="1"/>
@@ -13258,7 +13468,7 @@
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J12" s="5">
         <f t="shared" si="1"/>
@@ -13303,7 +13513,7 @@
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J13" s="5">
         <f t="shared" si="1"/>
@@ -13348,7 +13558,7 @@
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J14" s="5">
         <f t="shared" si="1"/>
@@ -13393,7 +13603,7 @@
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J15" s="5">
         <f t="shared" si="1"/>
@@ -13438,7 +13648,7 @@
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J16" s="5">
         <f t="shared" si="1"/>
@@ -13483,7 +13693,7 @@
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J17" s="5">
         <f t="shared" si="1"/>
@@ -13528,7 +13738,7 @@
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J18" s="5">
         <f t="shared" si="1"/>
@@ -13573,7 +13783,7 @@
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J19" s="5">
         <f t="shared" si="1"/>
@@ -13618,7 +13828,7 @@
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J20" s="5">
         <f t="shared" si="1"/>
@@ -13663,7 +13873,7 @@
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J21" s="5">
         <f t="shared" si="1"/>
@@ -13708,7 +13918,7 @@
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J22" s="5">
         <f t="shared" si="1"/>
@@ -13753,7 +13963,7 @@
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J23" s="5">
         <f t="shared" si="1"/>
@@ -13798,7 +14008,7 @@
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J24" s="5">
         <f t="shared" si="1"/>
@@ -13843,7 +14053,7 @@
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J25" s="5">
         <f t="shared" si="1"/>
@@ -13888,7 +14098,7 @@
       </c>
       <c r="H26" s="4"/>
       <c r="I26" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J26" s="5">
         <f t="shared" si="1"/>
@@ -13933,7 +14143,7 @@
       </c>
       <c r="H27" s="4"/>
       <c r="I27" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J27" s="5">
         <f t="shared" si="1"/>
@@ -13978,7 +14188,7 @@
       </c>
       <c r="H28" s="4"/>
       <c r="I28" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J28" s="5">
         <f t="shared" si="1"/>
@@ -14023,7 +14233,7 @@
       </c>
       <c r="H29" s="4"/>
       <c r="I29" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J29" s="5">
         <f t="shared" si="1"/>
@@ -14068,7 +14278,7 @@
       </c>
       <c r="H30" s="4"/>
       <c r="I30" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J30" s="5">
         <f t="shared" si="1"/>
@@ -14113,7 +14323,7 @@
       </c>
       <c r="H31" s="4"/>
       <c r="I31" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J31" s="5">
         <f t="shared" si="1"/>
@@ -14158,7 +14368,7 @@
       </c>
       <c r="H32" s="4"/>
       <c r="I32" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J32" s="5">
         <f t="shared" si="1"/>
@@ -14203,7 +14413,7 @@
       </c>
       <c r="H33" s="4"/>
       <c r="I33" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J33" s="5">
         <f t="shared" si="1"/>
@@ -14248,7 +14458,7 @@
       </c>
       <c r="H34" s="4"/>
       <c r="I34" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J34" s="5">
         <f t="shared" si="1"/>
@@ -14293,7 +14503,7 @@
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J35" s="5">
         <f t="shared" si="1"/>
@@ -14338,7 +14548,7 @@
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J36" s="5">
         <f t="shared" si="1"/>
@@ -14383,7 +14593,7 @@
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J37" s="5">
         <f t="shared" si="1"/>
@@ -14428,7 +14638,7 @@
       </c>
       <c r="H38" s="4"/>
       <c r="I38" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J38" s="5">
         <f t="shared" si="1"/>
@@ -14473,7 +14683,7 @@
       </c>
       <c r="H39" s="4"/>
       <c r="I39" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J39" s="5">
         <f t="shared" si="1"/>
@@ -14518,7 +14728,7 @@
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J40" s="5">
         <f t="shared" si="1"/>
@@ -14563,7 +14773,7 @@
       </c>
       <c r="H41" s="4"/>
       <c r="I41" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J41" s="5">
         <f t="shared" si="1"/>
@@ -14608,7 +14818,7 @@
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J42" s="5">
         <f t="shared" si="1"/>
@@ -14653,7 +14863,7 @@
       </c>
       <c r="H43" s="4"/>
       <c r="I43" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J43" s="5">
         <f t="shared" si="1"/>
@@ -14698,7 +14908,7 @@
       </c>
       <c r="H44" s="4"/>
       <c r="I44" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J44" s="5">
         <f t="shared" si="1"/>
@@ -14743,7 +14953,7 @@
       </c>
       <c r="H45" s="4"/>
       <c r="I45" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J45" s="5">
         <f t="shared" si="1"/>
@@ -14788,7 +14998,7 @@
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J46" s="5">
         <f t="shared" si="1"/>
@@ -14833,7 +15043,7 @@
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J47" s="5">
         <f t="shared" si="1"/>
@@ -14878,7 +15088,7 @@
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J48" s="5">
         <f t="shared" si="1"/>
@@ -14905,11 +15115,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -14970,19 +15180,19 @@
         <v>10</v>
       </c>
       <c r="S1" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="T1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U1" t="s">
         <v>62</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>63</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>64</v>
-      </c>
-      <c r="W1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:23">
@@ -15038,7 +15248,7 @@
         <v>18305</v>
       </c>
       <c r="Q2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R2">
         <f>B2</f>
@@ -15118,7 +15328,7 @@
         <v>52225</v>
       </c>
       <c r="Q3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R3">
         <f t="shared" ref="R3:R13" si="6">B3</f>
@@ -15198,7 +15408,7 @@
         <v>84240</v>
       </c>
       <c r="Q4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R4">
         <f t="shared" si="6"/>
@@ -15278,7 +15488,7 @@
         <v>196655</v>
       </c>
       <c r="Q5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R5">
         <f t="shared" si="6"/>
@@ -15358,7 +15568,7 @@
         <v>187445</v>
       </c>
       <c r="Q6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R6">
         <f t="shared" si="6"/>
@@ -15438,7 +15648,7 @@
         <v>393995</v>
       </c>
       <c r="Q7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R7">
         <f t="shared" si="6"/>
@@ -15518,7 +15728,7 @@
         <v>57745</v>
       </c>
       <c r="Q8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R8">
         <f t="shared" si="6"/>
@@ -15598,7 +15808,7 @@
         <v>117969</v>
       </c>
       <c r="Q9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R9">
         <f t="shared" si="6"/>
@@ -15678,7 +15888,7 @@
         <v>141100</v>
       </c>
       <c r="Q10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R10">
         <f t="shared" si="6"/>
@@ -15758,7 +15968,7 @@
         <v>230735</v>
       </c>
       <c r="Q11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R11">
         <f t="shared" si="6"/>
@@ -15806,26 +16016,26 @@
         <v>74.575000000000003</v>
       </c>
       <c r="Q12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R12">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="S12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="T12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="V12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="W12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:23">
@@ -15881,7 +16091,7 @@
         <v>461035</v>
       </c>
       <c r="Q13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R13">
         <f t="shared" si="6"/>

</xml_diff>

<commit_message>
more validation work for eucalyptus
</commit_message>
<xml_diff>
--- a/Prototypes/Egrandis/EucalyptusValidationData.xlsx
+++ b/Prototypes/Egrandis/EucalyptusValidationData.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="82">
   <si>
     <t>lai</t>
   </si>
@@ -276,9 +276,6 @@
     <t>Eucalyptus.Branch.Live.Wt</t>
   </si>
   <si>
-    <t>Eucalyptus.Wood.Live.Wt</t>
-  </si>
-  <si>
     <t>GympieIrrZeroNZero</t>
   </si>
   <si>
@@ -292,6 +289,12 @@
   </si>
   <si>
     <t>Eucalyptus.Leaf.LAI</t>
+  </si>
+  <si>
+    <t>Eucalyptus.Wood.Wt</t>
+  </si>
+  <si>
+    <t>Litterfall</t>
   </si>
 </sst>
 </file>
@@ -11503,1594 +11506,1642 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="J2" sqref="J2:J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
   <cols>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>0.25205479452054796</v>
       </c>
       <c r="B2" s="3">
         <v>33511</v>
       </c>
-      <c r="C2">
-        <v>1E-3</v>
-      </c>
+      <c r="C2" s="3"/>
       <c r="D2">
         <v>1E-3</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="E2">
+        <v>1E-3</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <f>A2</f>
         <v>0.25205479452054796</v>
       </c>
-      <c r="H2" s="5">
+      <c r="I2" s="5">
         <f>B2</f>
         <v>33511</v>
-      </c>
-      <c r="I2">
-        <f>C2</f>
-        <v>1E-3</v>
       </c>
       <c r="J2">
         <f>D2</f>
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2">
+        <f>E2</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>0.33698630136986302</v>
       </c>
       <c r="B3" s="3">
         <v>33542</v>
       </c>
-      <c r="C3">
-        <v>1E-3</v>
-      </c>
+      <c r="C3" s="3"/>
       <c r="D3">
         <v>1E-3</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="E3">
+        <v>1E-3</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G48" si="0">A3</f>
+      <c r="H3">
+        <f t="shared" ref="H3:H48" si="0">A3</f>
         <v>0.33698630136986302</v>
       </c>
-      <c r="H3" s="5">
-        <f t="shared" ref="H3:H48" si="1">B3</f>
+      <c r="I3" s="5">
+        <f t="shared" ref="I3:I48" si="1">B3</f>
         <v>33542</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:J48" si="2">C3</f>
+      <c r="J3">
+        <f t="shared" ref="J3:K48" si="2">D3</f>
         <v>1E-3</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>0.41917808219178082</v>
       </c>
       <c r="B4" s="3">
         <v>33572</v>
       </c>
-      <c r="C4">
-        <v>1E-3</v>
-      </c>
+      <c r="C4" s="3"/>
       <c r="D4">
         <v>1E-3</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="E4">
+        <v>1E-3</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <f t="shared" si="0"/>
         <v>0.41917808219178082</v>
       </c>
-      <c r="H4" s="5">
+      <c r="I4" s="5">
         <f t="shared" si="1"/>
         <v>33572</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>0.50410958904109593</v>
       </c>
       <c r="B5" s="3">
         <v>33603</v>
       </c>
-      <c r="C5">
-        <v>1E-3</v>
-      </c>
+      <c r="C5" s="3"/>
       <c r="D5">
         <v>1E-3</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="E5">
+        <v>1E-3</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <f t="shared" si="0"/>
         <v>0.50410958904109593</v>
       </c>
-      <c r="H5" s="5">
+      <c r="I5" s="5">
         <f t="shared" si="1"/>
         <v>33603</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>0.58904109589041098</v>
       </c>
       <c r="B6" s="3">
         <v>33634</v>
       </c>
-      <c r="C6">
-        <v>1E-3</v>
-      </c>
+      <c r="C6" s="3"/>
       <c r="D6">
         <v>1E-3</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="E6">
+        <v>1E-3</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <f t="shared" si="0"/>
         <v>0.58904109589041098</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6" s="5">
         <f t="shared" si="1"/>
         <v>33634</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>0.66849315068493154</v>
       </c>
       <c r="B7" s="3">
         <v>33663</v>
       </c>
-      <c r="C7">
-        <v>1E-3</v>
-      </c>
+      <c r="C7" s="3"/>
       <c r="D7">
         <v>1E-3</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="E7">
+        <v>1E-3</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <f t="shared" si="0"/>
         <v>0.66849315068493154</v>
       </c>
-      <c r="H7" s="5">
+      <c r="I7" s="5">
         <f t="shared" si="1"/>
         <v>33663</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>0.75342465753424659</v>
       </c>
       <c r="B8" s="3">
         <v>33694</v>
       </c>
-      <c r="C8">
-        <v>1E-3</v>
-      </c>
+      <c r="C8" s="3"/>
       <c r="D8">
         <v>1E-3</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="E8">
+        <v>1E-3</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <f t="shared" si="0"/>
         <v>0.75342465753424659</v>
       </c>
-      <c r="H8" s="5">
+      <c r="I8" s="5">
         <f t="shared" si="1"/>
         <v>33694</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>0.83561643835616439</v>
       </c>
       <c r="B9" s="3">
         <v>33724</v>
       </c>
-      <c r="C9">
-        <v>1E-3</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9">
         <v>1E-3</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="E9">
+        <v>1E-3</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <f t="shared" si="0"/>
         <v>0.83561643835616439</v>
       </c>
-      <c r="H9" s="5">
+      <c r="I9" s="5">
         <f t="shared" si="1"/>
         <v>33724</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>0.92054794520547945</v>
       </c>
       <c r="B10" s="3">
         <v>33755</v>
       </c>
-      <c r="C10">
-        <v>1E-3</v>
-      </c>
+      <c r="C10" s="3"/>
       <c r="D10">
         <v>1E-3</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="E10">
+        <v>1E-3</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <f t="shared" si="0"/>
         <v>0.92054794520547945</v>
       </c>
-      <c r="H10" s="5">
+      <c r="I10" s="5">
         <f t="shared" si="1"/>
         <v>33755</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>1.0027397260273974</v>
       </c>
       <c r="B11" s="3">
         <v>33785</v>
       </c>
-      <c r="C11">
-        <v>1E-3</v>
-      </c>
+      <c r="C11" s="3"/>
       <c r="D11">
         <v>1E-3</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="E11">
+        <v>1E-3</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <f t="shared" si="0"/>
         <v>1.0027397260273974</v>
       </c>
-      <c r="H11" s="5">
+      <c r="I11" s="5">
         <f t="shared" si="1"/>
         <v>33785</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>1.0876712328767124</v>
       </c>
       <c r="B12" s="3">
         <v>33816</v>
       </c>
-      <c r="C12">
-        <v>1E-3</v>
-      </c>
+      <c r="C12" s="3"/>
       <c r="D12">
         <v>1E-3</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="E12">
+        <v>1E-3</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <f t="shared" si="0"/>
         <v>1.0876712328767124</v>
       </c>
-      <c r="H12" s="5">
+      <c r="I12" s="5">
         <f t="shared" si="1"/>
         <v>33816</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>1.1726027397260275</v>
       </c>
       <c r="B13" s="3">
         <v>33847</v>
       </c>
-      <c r="C13">
-        <v>1E-3</v>
-      </c>
+      <c r="C13" s="3"/>
       <c r="D13">
         <v>1E-3</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="E13">
+        <v>1E-3</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <f t="shared" si="0"/>
         <v>1.1726027397260275</v>
       </c>
-      <c r="H13" s="5">
+      <c r="I13" s="5">
         <f t="shared" si="1"/>
         <v>33847</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>1.2547945205479452</v>
       </c>
       <c r="B14" s="3">
         <v>33877</v>
       </c>
-      <c r="C14">
-        <v>1E-3</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14">
         <v>1E-3</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="E14">
+        <v>1E-3</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <f t="shared" si="0"/>
         <v>1.2547945205479452</v>
       </c>
-      <c r="H14" s="5">
+      <c r="I14" s="5">
         <f t="shared" si="1"/>
         <v>33877</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>1.3397260273972602</v>
       </c>
       <c r="B15" s="3">
         <v>33908</v>
       </c>
-      <c r="C15">
-        <v>1E-3</v>
-      </c>
+      <c r="C15" s="3"/>
       <c r="D15">
         <v>1E-3</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="E15">
+        <v>1E-3</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <f t="shared" si="0"/>
         <v>1.3397260273972602</v>
       </c>
-      <c r="H15" s="5">
+      <c r="I15" s="5">
         <f t="shared" si="1"/>
         <v>33908</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>1.4219178082191781</v>
       </c>
       <c r="B16" s="3">
         <v>33938</v>
       </c>
-      <c r="C16">
-        <v>1E-3</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16">
         <v>1E-3</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="E16">
+        <v>1E-3</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <f t="shared" si="0"/>
         <v>1.4219178082191781</v>
       </c>
-      <c r="H16" s="5">
+      <c r="I16" s="5">
         <f t="shared" si="1"/>
         <v>33938</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>1.5068493150684932</v>
       </c>
       <c r="B17" s="3">
         <v>33969</v>
       </c>
-      <c r="C17">
-        <v>1E-3</v>
-      </c>
+      <c r="C17" s="3"/>
       <c r="D17">
         <v>1E-3</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="E17">
+        <v>1E-3</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <f t="shared" si="0"/>
         <v>1.5068493150684932</v>
       </c>
-      <c r="H17" s="5">
+      <c r="I17" s="5">
         <f t="shared" si="1"/>
         <v>33969</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>1.5917808219178082</v>
       </c>
       <c r="B18" s="3">
         <v>34000</v>
       </c>
-      <c r="C18">
-        <v>1E-3</v>
-      </c>
+      <c r="C18" s="3"/>
       <c r="D18">
         <v>1E-3</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="E18">
+        <v>1E-3</v>
+      </c>
+      <c r="G18" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <f t="shared" si="0"/>
         <v>1.5917808219178082</v>
       </c>
-      <c r="H18" s="5">
+      <c r="I18" s="5">
         <f t="shared" si="1"/>
         <v>34000</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>1.6684931506849314</v>
       </c>
       <c r="B19" s="3">
         <v>34028</v>
       </c>
-      <c r="C19">
-        <v>1E-3</v>
-      </c>
+      <c r="C19" s="3"/>
       <c r="D19">
         <v>1E-3</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="E19">
+        <v>1E-3</v>
+      </c>
+      <c r="G19" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <f t="shared" si="0"/>
         <v>1.6684931506849314</v>
       </c>
-      <c r="H19" s="5">
+      <c r="I19" s="5">
         <f t="shared" si="1"/>
         <v>34028</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>1.7534246575342465</v>
       </c>
       <c r="B20" s="3">
         <v>34059</v>
       </c>
-      <c r="C20">
-        <v>1E-3</v>
-      </c>
+      <c r="C20" s="3"/>
       <c r="D20">
         <v>1E-3</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="E20">
+        <v>1E-3</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <f t="shared" si="0"/>
         <v>1.7534246575342465</v>
       </c>
-      <c r="H20" s="5">
+      <c r="I20" s="5">
         <f t="shared" si="1"/>
         <v>34059</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>1.8356164383561644</v>
       </c>
       <c r="B21" s="3">
         <v>34089</v>
       </c>
-      <c r="C21">
-        <v>46.975000000000001</v>
-      </c>
+      <c r="C21" s="3"/>
       <c r="D21">
         <v>46.975000000000001</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="E21">
+        <v>46.975000000000001</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <f t="shared" si="0"/>
         <v>1.8356164383561644</v>
       </c>
-      <c r="H21" s="5">
+      <c r="I21" s="5">
         <f t="shared" si="1"/>
         <v>34089</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <f t="shared" si="2"/>
         <v>46.975000000000001</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <f t="shared" si="2"/>
         <v>46.975000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:11">
       <c r="A22">
         <v>1.9205479452054794</v>
       </c>
       <c r="B22" s="3">
         <v>34120</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="3"/>
+      <c r="D22">
         <v>39.375</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>86.35</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="G22" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <f t="shared" si="0"/>
         <v>1.9205479452054794</v>
       </c>
-      <c r="H22" s="5">
+      <c r="I22" s="5">
         <f t="shared" si="1"/>
         <v>34120</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <f t="shared" si="2"/>
         <v>39.375</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <f t="shared" si="2"/>
         <v>86.35</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:11">
       <c r="A23">
         <v>2.0027397260273974</v>
       </c>
       <c r="B23" s="3">
         <v>34150</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="3"/>
+      <c r="D23">
         <v>32.549999999999997</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>118.9</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="G23" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <f t="shared" si="0"/>
         <v>2.0027397260273974</v>
       </c>
-      <c r="H23" s="5">
+      <c r="I23" s="5">
         <f t="shared" si="1"/>
         <v>34150</v>
       </c>
-      <c r="I23">
+      <c r="J23">
         <f t="shared" si="2"/>
         <v>32.549999999999997</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <f t="shared" si="2"/>
         <v>118.9</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:11">
       <c r="A24">
         <v>2.0876712328767124</v>
       </c>
       <c r="B24" s="3">
         <v>34181</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="3"/>
+      <c r="D24">
         <v>25.912500000000001</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>144.8125</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="G24" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <f t="shared" si="0"/>
         <v>2.0876712328767124</v>
       </c>
-      <c r="H24" s="5">
+      <c r="I24" s="5">
         <f t="shared" si="1"/>
         <v>34181</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <f t="shared" si="2"/>
         <v>25.912500000000001</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <f t="shared" si="2"/>
         <v>144.8125</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>2.1726027397260275</v>
       </c>
       <c r="B25" s="3">
         <v>34212</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="3"/>
+      <c r="D25">
         <v>47.25</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>192.0625</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="G25" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <f t="shared" si="0"/>
         <v>2.1726027397260275</v>
       </c>
-      <c r="H25" s="5">
+      <c r="I25" s="5">
         <f t="shared" si="1"/>
         <v>34212</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <f t="shared" si="2"/>
         <v>47.25</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <f t="shared" si="2"/>
         <v>192.0625</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>2.2547945205479452</v>
       </c>
       <c r="B26" s="3">
         <v>34242</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="3"/>
+      <c r="D26">
         <v>97.912499999999994</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>289.97500000000002</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="G26" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <f t="shared" si="0"/>
         <v>2.2547945205479452</v>
       </c>
-      <c r="H26" s="5">
+      <c r="I26" s="5">
         <f t="shared" si="1"/>
         <v>34242</v>
       </c>
-      <c r="I26">
+      <c r="J26">
         <f t="shared" si="2"/>
         <v>97.912499999999994</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <f t="shared" si="2"/>
         <v>289.97500000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:11">
       <c r="A27">
         <v>2.3397260273972602</v>
       </c>
       <c r="B27" s="3">
         <v>34273</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="3"/>
+      <c r="D27">
         <v>221.625</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>511.6</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="G27" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <f t="shared" si="0"/>
         <v>2.3397260273972602</v>
       </c>
-      <c r="H27" s="5">
+      <c r="I27" s="5">
         <f t="shared" si="1"/>
         <v>34273</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <f t="shared" si="2"/>
         <v>221.625</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <f t="shared" si="2"/>
         <v>511.6</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:11">
       <c r="A28">
         <v>2.4219178082191779</v>
       </c>
       <c r="B28" s="3">
         <v>34303</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="3"/>
+      <c r="D28">
         <v>616.45000000000005</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>1128.05</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="G28" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <f t="shared" si="0"/>
         <v>2.4219178082191779</v>
       </c>
-      <c r="H28" s="5">
+      <c r="I28" s="5">
         <f t="shared" si="1"/>
         <v>34303</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <f t="shared" si="2"/>
         <v>616.45000000000005</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <f t="shared" si="2"/>
         <v>1128.05</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:11">
       <c r="A29">
         <v>2.506849315068493</v>
       </c>
       <c r="B29" s="3">
         <v>34334</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="3"/>
+      <c r="D29">
         <v>924.52499999999998</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>2052.5749999999998</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="G29" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <f t="shared" si="0"/>
         <v>2.506849315068493</v>
       </c>
-      <c r="H29" s="5">
+      <c r="I29" s="5">
         <f t="shared" si="1"/>
         <v>34334</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <f t="shared" si="2"/>
         <v>924.52499999999998</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <f t="shared" si="2"/>
         <v>2052.5749999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:11">
       <c r="A30">
         <v>2.591780821917808</v>
       </c>
       <c r="B30" s="3">
         <v>34365</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="3"/>
+      <c r="D30">
         <v>932.98749999999995</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>2985.5625</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="G30" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <f t="shared" si="0"/>
         <v>2.591780821917808</v>
       </c>
-      <c r="H30" s="5">
+      <c r="I30" s="5">
         <f t="shared" si="1"/>
         <v>34365</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <f t="shared" si="2"/>
         <v>932.98749999999995</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <f t="shared" si="2"/>
         <v>2985.5625</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:11">
       <c r="A31">
         <v>2.6684931506849314</v>
       </c>
       <c r="B31" s="3">
         <v>34393</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="3"/>
+      <c r="D31">
         <v>722.83749999999998</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>3708.4</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="G31" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <f t="shared" si="0"/>
         <v>2.6684931506849314</v>
       </c>
-      <c r="H31" s="5">
+      <c r="I31" s="5">
         <f t="shared" si="1"/>
         <v>34393</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <f t="shared" si="2"/>
         <v>722.83749999999998</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <f t="shared" si="2"/>
         <v>3708.4</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:11">
       <c r="A32">
         <v>2.7534246575342465</v>
       </c>
       <c r="B32" s="3">
         <v>34424</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="3"/>
+      <c r="D32">
         <v>403.66250000000002</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>4112.0625</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="G32" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <f t="shared" si="0"/>
         <v>2.7534246575342465</v>
       </c>
-      <c r="H32" s="5">
+      <c r="I32" s="5">
         <f t="shared" si="1"/>
         <v>34424</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <f t="shared" si="2"/>
         <v>403.66250000000002</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <f t="shared" si="2"/>
         <v>4112.0625</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:11">
       <c r="A33">
         <v>2.8356164383561642</v>
       </c>
       <c r="B33" s="3">
         <v>34454</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="3"/>
+      <c r="D33">
         <v>321.52499999999998</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>4433.5874999999996</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="G33" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <f t="shared" si="0"/>
         <v>2.8356164383561642</v>
       </c>
-      <c r="H33" s="5">
+      <c r="I33" s="5">
         <f t="shared" si="1"/>
         <v>34454</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <f t="shared" si="2"/>
         <v>321.52499999999998</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <f t="shared" si="2"/>
         <v>4433.5874999999996</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:11">
       <c r="A34">
         <v>2.9205479452054797</v>
       </c>
       <c r="B34" s="3">
         <v>34485</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="3"/>
+      <c r="D34">
         <v>212.3125</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>4645.8999999999996</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="G34" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <f t="shared" si="0"/>
         <v>2.9205479452054797</v>
       </c>
-      <c r="H34" s="5">
+      <c r="I34" s="5">
         <f t="shared" si="1"/>
         <v>34485</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <f t="shared" si="2"/>
         <v>212.3125</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <f t="shared" si="2"/>
         <v>4645.8999999999996</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:11">
       <c r="A35">
         <v>3.0027397260273974</v>
       </c>
       <c r="B35" s="3">
         <v>34515</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="3"/>
+      <c r="D35">
         <v>100.175</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>4746.0749999999998</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="G35" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <f t="shared" si="0"/>
         <v>3.0027397260273974</v>
       </c>
-      <c r="H35" s="5">
+      <c r="I35" s="5">
         <f t="shared" si="1"/>
         <v>34515</v>
       </c>
-      <c r="I35">
+      <c r="J35">
         <f t="shared" si="2"/>
         <v>100.175</v>
       </c>
-      <c r="J35">
+      <c r="K35">
         <f t="shared" si="2"/>
         <v>4746.0749999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:11">
       <c r="A36">
         <v>3.0876712328767124</v>
       </c>
       <c r="B36" s="3">
         <v>34546</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="3"/>
+      <c r="D36">
         <v>63.5625</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>4809.6374999999998</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="G36" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <f t="shared" si="0"/>
         <v>3.0876712328767124</v>
       </c>
-      <c r="H36" s="5">
+      <c r="I36" s="5">
         <f t="shared" si="1"/>
         <v>34546</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <f t="shared" si="2"/>
         <v>63.5625</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <f t="shared" si="2"/>
         <v>4809.6374999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:11">
       <c r="A37">
         <v>3.1726027397260275</v>
       </c>
       <c r="B37" s="3">
         <v>34577</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="3"/>
+      <c r="D37">
         <v>155.08750000000001</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>4964.7249999999995</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="G37" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <f t="shared" si="0"/>
         <v>3.1726027397260275</v>
       </c>
-      <c r="H37" s="5">
+      <c r="I37" s="5">
         <f t="shared" si="1"/>
         <v>34577</v>
       </c>
-      <c r="I37">
+      <c r="J37">
         <f t="shared" si="2"/>
         <v>155.08750000000001</v>
       </c>
-      <c r="J37">
+      <c r="K37">
         <f t="shared" si="2"/>
         <v>4964.7249999999995</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:11">
       <c r="A38">
         <v>3.2547945205479452</v>
       </c>
       <c r="B38" s="3">
         <v>34607</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="3"/>
+      <c r="D38">
         <v>219.63749999999999</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>5184.3624999999993</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="G38" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <f t="shared" si="0"/>
         <v>3.2547945205479452</v>
       </c>
-      <c r="H38" s="5">
+      <c r="I38" s="5">
         <f t="shared" si="1"/>
         <v>34607</v>
       </c>
-      <c r="I38">
+      <c r="J38">
         <f t="shared" si="2"/>
         <v>219.63749999999999</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <f t="shared" si="2"/>
         <v>5184.3624999999993</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:11">
       <c r="A39">
         <v>3.3397260273972602</v>
       </c>
       <c r="B39" s="3">
         <v>34638</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="3"/>
+      <c r="D39">
         <v>420.75</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>5605.1124999999993</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="G39" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <f t="shared" si="0"/>
         <v>3.3397260273972602</v>
       </c>
-      <c r="H39" s="5">
+      <c r="I39" s="5">
         <f t="shared" si="1"/>
         <v>34638</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <f t="shared" si="2"/>
         <v>420.75</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <f t="shared" si="2"/>
         <v>5605.1124999999993</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:11">
       <c r="A40">
         <v>3.4219178082191779</v>
       </c>
       <c r="B40" s="3">
         <v>34668</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="3"/>
+      <c r="D40">
         <v>660.27499999999998</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>6265.3874999999989</v>
       </c>
-      <c r="F40" s="7" t="s">
+      <c r="G40" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <f t="shared" si="0"/>
         <v>3.4219178082191779</v>
       </c>
-      <c r="H40" s="5">
+      <c r="I40" s="5">
         <f t="shared" si="1"/>
         <v>34668</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <f t="shared" si="2"/>
         <v>660.27499999999998</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <f t="shared" si="2"/>
         <v>6265.3874999999989</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:11">
       <c r="A41">
         <v>3.506849315068493</v>
       </c>
       <c r="B41" s="3">
         <v>34699</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="3"/>
+      <c r="D41">
         <v>1338.4375000000002</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>7603.8249999999989</v>
       </c>
-      <c r="F41" s="7" t="s">
+      <c r="G41" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <f t="shared" si="0"/>
         <v>3.506849315068493</v>
       </c>
-      <c r="H41" s="5">
+      <c r="I41" s="5">
         <f t="shared" si="1"/>
         <v>34699</v>
       </c>
-      <c r="I41">
+      <c r="J41">
         <f t="shared" si="2"/>
         <v>1338.4375000000002</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <f t="shared" si="2"/>
         <v>7603.8249999999989</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:11">
       <c r="A42">
         <v>3.591780821917808</v>
       </c>
       <c r="B42" s="3">
         <v>34730</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="3"/>
+      <c r="D42">
         <v>548.4</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>8152.2249999999985</v>
       </c>
-      <c r="F42" s="7" t="s">
+      <c r="G42" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <f t="shared" si="0"/>
         <v>3.591780821917808</v>
       </c>
-      <c r="H42" s="5">
+      <c r="I42" s="5">
         <f t="shared" si="1"/>
         <v>34730</v>
       </c>
-      <c r="I42">
+      <c r="J42">
         <f t="shared" si="2"/>
         <v>548.4</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <f t="shared" si="2"/>
         <v>8152.2249999999985</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:11">
       <c r="A43">
         <v>3.6684931506849314</v>
       </c>
       <c r="B43" s="3">
         <v>34758</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="3"/>
+      <c r="D43">
         <v>377.16250000000002</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>8529.3874999999989</v>
       </c>
-      <c r="F43" s="7" t="s">
+      <c r="G43" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <f t="shared" si="0"/>
         <v>3.6684931506849314</v>
       </c>
-      <c r="H43" s="5">
+      <c r="I43" s="5">
         <f t="shared" si="1"/>
         <v>34758</v>
       </c>
-      <c r="I43">
+      <c r="J43">
         <f t="shared" si="2"/>
         <v>377.16250000000002</v>
       </c>
-      <c r="J43">
+      <c r="K43">
         <f t="shared" si="2"/>
         <v>8529.3874999999989</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:11">
       <c r="A44">
         <v>3.7534246575342465</v>
       </c>
       <c r="B44" s="3">
         <v>34789</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="3"/>
+      <c r="D44">
         <v>655.04999999999995</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>9184.4374999999982</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="G44" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <f t="shared" si="0"/>
         <v>3.7534246575342465</v>
       </c>
-      <c r="H44" s="5">
+      <c r="I44" s="5">
         <f t="shared" si="1"/>
         <v>34789</v>
       </c>
-      <c r="I44">
+      <c r="J44">
         <f t="shared" si="2"/>
         <v>655.04999999999995</v>
       </c>
-      <c r="J44">
+      <c r="K44">
         <f t="shared" si="2"/>
         <v>9184.4374999999982</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:11">
       <c r="A45">
         <v>3.8356164383561642</v>
       </c>
       <c r="B45" s="3">
         <v>34819</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="3"/>
+      <c r="D45">
         <v>259.92500000000001</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>9444.3624999999975</v>
       </c>
-      <c r="F45" s="7" t="s">
+      <c r="G45" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <f t="shared" si="0"/>
         <v>3.8356164383561642</v>
       </c>
-      <c r="H45" s="5">
+      <c r="I45" s="5">
         <f t="shared" si="1"/>
         <v>34819</v>
       </c>
-      <c r="I45">
+      <c r="J45">
         <f t="shared" si="2"/>
         <v>259.92500000000001</v>
       </c>
-      <c r="J45">
+      <c r="K45">
         <f t="shared" si="2"/>
         <v>9444.3624999999975</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:11">
       <c r="A46">
         <v>3.9205479452054797</v>
       </c>
       <c r="B46" s="3">
         <v>34850</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="3"/>
+      <c r="D46">
         <v>204.9375</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>9649.2999999999993</v>
       </c>
-      <c r="F46" s="7" t="s">
+      <c r="G46" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G46">
+      <c r="H46">
         <f t="shared" si="0"/>
         <v>3.9205479452054797</v>
       </c>
-      <c r="H46" s="5">
+      <c r="I46" s="5">
         <f t="shared" si="1"/>
         <v>34850</v>
       </c>
-      <c r="I46">
+      <c r="J46">
         <f t="shared" si="2"/>
         <v>204.9375</v>
       </c>
-      <c r="J46">
+      <c r="K46">
         <f t="shared" si="2"/>
         <v>9649.2999999999993</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:11">
       <c r="A47">
         <v>4.0027397260273974</v>
       </c>
       <c r="B47" s="3">
         <v>34880</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="3"/>
+      <c r="D47">
         <v>118.7375</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>9768.0374999999967</v>
       </c>
-      <c r="F47" s="7" t="s">
+      <c r="G47" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <f t="shared" si="0"/>
         <v>4.0027397260273974</v>
       </c>
-      <c r="H47" s="5">
+      <c r="I47" s="5">
         <f t="shared" si="1"/>
         <v>34880</v>
       </c>
-      <c r="I47">
+      <c r="J47">
         <f t="shared" si="2"/>
         <v>118.7375</v>
       </c>
-      <c r="J47">
+      <c r="K47">
         <f t="shared" si="2"/>
         <v>9768.0374999999967</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:11">
       <c r="A48">
         <v>4.087671232876712</v>
       </c>
       <c r="B48" s="3">
         <v>34911</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="3"/>
+      <c r="D48">
         <v>52.5625</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>9820.6</v>
       </c>
-      <c r="F48" s="7" t="s">
+      <c r="G48" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <f t="shared" si="0"/>
         <v>4.087671232876712</v>
       </c>
-      <c r="H48" s="5">
+      <c r="I48" s="5">
         <f t="shared" si="1"/>
         <v>34911</v>
       </c>
-      <c r="I48">
+      <c r="J48">
         <f t="shared" si="2"/>
         <v>52.5625</v>
       </c>
-      <c r="J48">
+      <c r="K48">
         <f t="shared" si="2"/>
         <v>9820.6</v>
       </c>
@@ -13106,8 +13157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
@@ -15283,7 +15334,7 @@
   <dimension ref="A1:W13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="D2:G2"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
@@ -16291,10 +16342,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="E88" workbookViewId="0">
+      <selection activeCell="K54" sqref="K54:K100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
@@ -16307,9 +16358,10 @@
     <col min="7" max="7" width="20.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.71875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -16323,7 +16375,7 @@
         <v>71</v>
       </c>
       <c r="E1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F1" t="s">
         <v>69</v>
@@ -16338,10 +16390,13 @@
         <v>74</v>
       </c>
       <c r="J1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>79</v>
+      </c>
+      <c r="K1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -16378,7 +16433,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -16415,7 +16470,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -16452,7 +16507,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -16489,7 +16544,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -16526,7 +16581,7 @@
         <v>1777.5</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -16563,7 +16618,7 @@
         <v>2083.5</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -16600,7 +16655,7 @@
         <v>1855</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -16637,7 +16692,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -16674,7 +16729,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -16711,7 +16766,7 @@
         <v>1735</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -16723,16 +16778,8 @@
         <f>CoffsBiomass!B12</f>
         <v>20</v>
       </c>
-      <c r="E12">
-        <f t="shared" si="1"/>
-        <v>7457.5</v>
-      </c>
-      <c r="F12">
-        <f>CoffsBiomass!H12*1000/10</f>
-        <v>7457.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -16769,9 +16816,9 @@
         <v>2207.5</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" s="10">
         <v>32052.9</v>
@@ -16802,9 +16849,9 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" s="10">
         <v>32191.599999999999</v>
@@ -16835,9 +16882,9 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="10">
         <v>32337.599999999999</v>
@@ -16870,7 +16917,7 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B17" s="10">
         <v>32472.65</v>
@@ -16903,7 +16950,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" s="10">
         <v>32688</v>
@@ -16936,7 +16983,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B19" s="10">
         <v>32943.5</v>
@@ -16969,7 +17016,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B20" s="10">
         <v>33126</v>
@@ -17002,7 +17049,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B21" s="10">
         <v>33308.5</v>
@@ -17035,7 +17082,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" s="10">
         <v>33491</v>
@@ -17068,7 +17115,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B23" s="10">
         <v>33856</v>
@@ -17101,7 +17148,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" s="10">
         <v>32052.9</v>
@@ -17134,7 +17181,7 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" s="10">
         <v>32191.599999999999</v>
@@ -17167,7 +17214,7 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B26" s="10">
         <v>32337.599999999999</v>
@@ -17200,7 +17247,7 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B27" s="10">
         <v>32472.65</v>
@@ -17233,7 +17280,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B28" s="10">
         <v>32688</v>
@@ -17266,7 +17313,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="10">
         <v>32943.5</v>
@@ -17299,7 +17346,7 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" s="10">
         <v>33126</v>
@@ -17332,7 +17379,7 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31" s="10">
         <v>33308.5</v>
@@ -17365,7 +17412,7 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B32" s="10">
         <v>33491</v>
@@ -17398,7 +17445,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B33" s="10">
         <v>33856</v>
@@ -17431,7 +17478,7 @@
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B34" s="10">
         <v>32052.9</v>
@@ -17464,7 +17511,7 @@
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B35" s="10">
         <v>32191.599999999999</v>
@@ -17497,7 +17544,7 @@
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="10">
         <v>32337.599999999999</v>
@@ -17530,7 +17577,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B37" s="10">
         <v>32472.65</v>
@@ -17563,7 +17610,7 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B38" s="10">
         <v>32688</v>
@@ -17596,7 +17643,7 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B39" s="10">
         <v>32943.5</v>
@@ -17629,7 +17676,7 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B40" s="10">
         <v>33126</v>
@@ -17662,7 +17709,7 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B41" s="10">
         <v>33308.5</v>
@@ -17695,7 +17742,7 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B42" s="10">
         <v>33491</v>
@@ -17728,7 +17775,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B43" s="10">
         <v>33856</v>
@@ -17761,7 +17808,7 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B44" s="10">
         <v>32052.9</v>
@@ -17794,7 +17841,7 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B45" s="10">
         <v>32191.599999999999</v>
@@ -17827,7 +17874,7 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B46" s="10">
         <v>32337.599999999999</v>
@@ -17860,7 +17907,7 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B47" s="10">
         <v>32472.65</v>
@@ -17893,7 +17940,7 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B48" s="10">
         <v>32688</v>
@@ -17924,9 +17971,9 @@
         <v>3.87</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:11">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B49" s="10">
         <v>32943.5</v>
@@ -17957,9 +18004,9 @@
         <v>3.6865749439928703</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:11">
       <c r="A50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B50" s="10">
         <v>33126</v>
@@ -17990,9 +18037,9 @@
         <v>3.7855418070094617</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:11">
       <c r="A51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B51" s="10">
         <v>33308.5</v>
@@ -18023,9 +18070,9 @@
         <v>3.9889772338145639</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:11">
       <c r="A52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B52" s="10">
         <v>33491</v>
@@ -18056,9 +18103,9 @@
         <v>4.5351055053411846</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:11">
       <c r="A53" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B53" s="10">
         <v>33856</v>
@@ -18087,6 +18134,1416 @@
       </c>
       <c r="J53">
         <v>5.3922041846935125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54" s="3">
+        <v>33510</v>
+      </c>
+      <c r="C54">
+        <v>0.24929999999999999</v>
+      </c>
+      <c r="D54">
+        <f>WaggaBiomass!F2/10</f>
+        <v>1E-3</v>
+      </c>
+      <c r="E54">
+        <f>WaggaBiomass!G2/10</f>
+        <v>1E-3</v>
+      </c>
+      <c r="F54">
+        <f>D54+E54</f>
+        <v>2E-3</v>
+      </c>
+      <c r="J54" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="K54">
+        <f>Waggalitterfall!J2/10</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" s="3">
+        <v>33541</v>
+      </c>
+      <c r="C55">
+        <v>0.3342</v>
+      </c>
+      <c r="D55">
+        <f>WaggaBiomass!F3/10</f>
+        <v>5.3</v>
+      </c>
+      <c r="E55">
+        <f>WaggaBiomass!G3/10</f>
+        <v>4</v>
+      </c>
+      <c r="F55">
+        <f t="shared" ref="F55:F100" si="3">D55+E55</f>
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="J55" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="K55">
+        <f>Waggalitterfall!J3/10</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="3">
+        <v>33571</v>
+      </c>
+      <c r="C56">
+        <v>0.41639999999999999</v>
+      </c>
+      <c r="D56">
+        <f>WaggaBiomass!F4/10</f>
+        <v>10.6</v>
+      </c>
+      <c r="E56">
+        <f>WaggaBiomass!G4/10</f>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="3"/>
+        <v>19.299999999999997</v>
+      </c>
+      <c r="J56" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="K56">
+        <f>Waggalitterfall!J4/10</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" s="3">
+        <v>33603</v>
+      </c>
+      <c r="C57">
+        <v>0.50139999999999996</v>
+      </c>
+      <c r="D57">
+        <f>WaggaBiomass!F5/10</f>
+        <v>15.9</v>
+      </c>
+      <c r="E57">
+        <f>WaggaBiomass!G5/10</f>
+        <v>15.4</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="3"/>
+        <v>31.3</v>
+      </c>
+      <c r="J57" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="K57">
+        <f>Waggalitterfall!J5/10</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58" s="3">
+        <v>33633</v>
+      </c>
+      <c r="C58">
+        <v>0.58630000000000004</v>
+      </c>
+      <c r="D58">
+        <f>WaggaBiomass!F6/10</f>
+        <v>21.2</v>
+      </c>
+      <c r="E58">
+        <f>WaggaBiomass!G6/10</f>
+        <v>23.5</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="3"/>
+        <v>44.7</v>
+      </c>
+      <c r="J58" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="K58">
+        <f>Waggalitterfall!J6/10</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" s="3">
+        <v>33663</v>
+      </c>
+      <c r="C59">
+        <v>0.66579999999999995</v>
+      </c>
+      <c r="D59">
+        <f>WaggaBiomass!F7/10</f>
+        <v>26.5</v>
+      </c>
+      <c r="E59">
+        <f>WaggaBiomass!G7/10</f>
+        <v>33.5</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="J59" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="K59">
+        <f>Waggalitterfall!J7/10</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="3">
+        <v>33694</v>
+      </c>
+      <c r="C60">
+        <v>0.75070000000000003</v>
+      </c>
+      <c r="D60">
+        <f>WaggaBiomass!F8/10</f>
+        <v>31.8</v>
+      </c>
+      <c r="E60">
+        <f>WaggaBiomass!G8/10</f>
+        <v>43.6</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="3"/>
+        <v>75.400000000000006</v>
+      </c>
+      <c r="J60" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="K60">
+        <f>Waggalitterfall!J8/10</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" s="3">
+        <v>33724</v>
+      </c>
+      <c r="C61">
+        <v>0.83289999999999997</v>
+      </c>
+      <c r="D61">
+        <f>WaggaBiomass!F9/10</f>
+        <v>37.1</v>
+      </c>
+      <c r="E61">
+        <f>WaggaBiomass!G9/10</f>
+        <v>52.3</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="3"/>
+        <v>89.4</v>
+      </c>
+      <c r="J61" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="K61">
+        <f>Waggalitterfall!J9/10</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62" s="3">
+        <v>33754</v>
+      </c>
+      <c r="C62">
+        <v>0.91779999999999995</v>
+      </c>
+      <c r="D62">
+        <f>WaggaBiomass!F10/10</f>
+        <v>42.4</v>
+      </c>
+      <c r="E62">
+        <f>WaggaBiomass!G10/10</f>
+        <v>59</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="3"/>
+        <v>101.4</v>
+      </c>
+      <c r="J62" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K62">
+        <f>Waggalitterfall!J10/10</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" s="3">
+        <v>33785</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <f>WaggaBiomass!F11/10</f>
+        <v>47.7</v>
+      </c>
+      <c r="E63">
+        <f>WaggaBiomass!G11/10</f>
+        <v>64.3</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="3"/>
+        <v>112</v>
+      </c>
+      <c r="J63" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="K63">
+        <f>Waggalitterfall!J11/10</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" s="3">
+        <v>33815</v>
+      </c>
+      <c r="C64">
+        <v>1.0832999999999999</v>
+      </c>
+      <c r="D64">
+        <f>WaggaBiomass!F12/10</f>
+        <v>53</v>
+      </c>
+      <c r="E64">
+        <f>WaggaBiomass!G12/10</f>
+        <v>67</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="3"/>
+        <v>120</v>
+      </c>
+      <c r="J64" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="K64">
+        <f>Waggalitterfall!J12/10</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" s="3">
+        <v>33846</v>
+      </c>
+      <c r="C65">
+        <v>1.1679999999999999</v>
+      </c>
+      <c r="D65">
+        <f>WaggaBiomass!F13/10</f>
+        <v>77.7</v>
+      </c>
+      <c r="E65">
+        <f>WaggaBiomass!G13/10</f>
+        <v>97</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="3"/>
+        <v>174.7</v>
+      </c>
+      <c r="J65" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="K65">
+        <f>Waggalitterfall!J13/10</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" s="3">
+        <v>33876</v>
+      </c>
+      <c r="C66">
+        <v>1.25</v>
+      </c>
+      <c r="D66">
+        <f>WaggaBiomass!F14/10</f>
+        <v>102.3</v>
+      </c>
+      <c r="E66">
+        <f>WaggaBiomass!G14/10</f>
+        <v>126.9</v>
+      </c>
+      <c r="F66">
+        <f t="shared" si="3"/>
+        <v>229.2</v>
+      </c>
+      <c r="J66" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="K66">
+        <f>Waggalitterfall!J14/10</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67" s="3">
+        <v>33907</v>
+      </c>
+      <c r="C67">
+        <v>1.3347</v>
+      </c>
+      <c r="D67">
+        <f>WaggaBiomass!F15/10</f>
+        <v>127</v>
+      </c>
+      <c r="E67">
+        <f>WaggaBiomass!G15/10</f>
+        <v>169.7</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="3"/>
+        <v>296.7</v>
+      </c>
+      <c r="J67" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="K67">
+        <f>Waggalitterfall!J15/10</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68" t="s">
+        <v>66</v>
+      </c>
+      <c r="B68" s="3">
+        <v>33937</v>
+      </c>
+      <c r="C68">
+        <v>1.4167000000000001</v>
+      </c>
+      <c r="D68">
+        <f>WaggaBiomass!F16/10</f>
+        <v>151.69999999999999</v>
+      </c>
+      <c r="E68">
+        <f>WaggaBiomass!G16/10</f>
+        <v>221.9</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="3"/>
+        <v>373.6</v>
+      </c>
+      <c r="J68" s="4">
+        <v>1.7</v>
+      </c>
+      <c r="K68">
+        <f>Waggalitterfall!J16/10</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" t="s">
+        <v>66</v>
+      </c>
+      <c r="B69" s="3">
+        <v>33968</v>
+      </c>
+      <c r="C69">
+        <v>1.5014000000000001</v>
+      </c>
+      <c r="D69">
+        <f>WaggaBiomass!F17/10</f>
+        <v>176.3</v>
+      </c>
+      <c r="E69">
+        <f>WaggaBiomass!G17/10</f>
+        <v>292</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="3"/>
+        <v>468.3</v>
+      </c>
+      <c r="J69" s="4">
+        <v>2</v>
+      </c>
+      <c r="K69">
+        <f>Waggalitterfall!J17/10</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" t="s">
+        <v>66</v>
+      </c>
+      <c r="B70" s="3">
+        <v>33998</v>
+      </c>
+      <c r="C70">
+        <v>1.5861000000000001</v>
+      </c>
+      <c r="D70">
+        <f>WaggaBiomass!F18/10</f>
+        <v>201</v>
+      </c>
+      <c r="E70">
+        <f>WaggaBiomass!G18/10</f>
+        <v>373</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="3"/>
+        <v>574</v>
+      </c>
+      <c r="J70" s="4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="K70">
+        <f>Waggalitterfall!J18/10</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" t="s">
+        <v>66</v>
+      </c>
+      <c r="B71" s="3">
+        <v>34026</v>
+      </c>
+      <c r="C71">
+        <v>1.6626000000000001</v>
+      </c>
+      <c r="D71">
+        <f>WaggaBiomass!F19/10</f>
+        <v>294.39999999999998</v>
+      </c>
+      <c r="E71">
+        <f>WaggaBiomass!G19/10</f>
+        <v>565</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="3"/>
+        <v>859.4</v>
+      </c>
+      <c r="J71" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="K71">
+        <f>Waggalitterfall!J19/10</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" t="s">
+        <v>66</v>
+      </c>
+      <c r="B72" s="3">
+        <v>34057</v>
+      </c>
+      <c r="C72">
+        <v>1.7473000000000001</v>
+      </c>
+      <c r="D72">
+        <f>WaggaBiomass!F20/10</f>
+        <v>342.5</v>
+      </c>
+      <c r="E72">
+        <f>WaggaBiomass!G20/10</f>
+        <v>765.2</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="3"/>
+        <v>1107.7</v>
+      </c>
+      <c r="J72" s="4">
+        <v>3.2</v>
+      </c>
+      <c r="K72">
+        <f>Waggalitterfall!J20/10</f>
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" t="s">
+        <v>66</v>
+      </c>
+      <c r="B73" s="3">
+        <v>34087</v>
+      </c>
+      <c r="C73">
+        <v>1.8291999999999999</v>
+      </c>
+      <c r="D73">
+        <f>WaggaBiomass!F21/10</f>
+        <v>387.8</v>
+      </c>
+      <c r="E73">
+        <f>WaggaBiomass!G21/10</f>
+        <v>926.2</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="3"/>
+        <v>1314</v>
+      </c>
+      <c r="J73" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="K73">
+        <f>Waggalitterfall!J21/10</f>
+        <v>4.6974999999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74" t="s">
+        <v>66</v>
+      </c>
+      <c r="B74" s="3">
+        <v>34118</v>
+      </c>
+      <c r="C74">
+        <v>1.9138999999999999</v>
+      </c>
+      <c r="D74">
+        <f>WaggaBiomass!F22/10</f>
+        <v>413.3</v>
+      </c>
+      <c r="E74">
+        <f>WaggaBiomass!G22/10</f>
+        <v>1046.8</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="3"/>
+        <v>1460.1</v>
+      </c>
+      <c r="J74" s="4">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="K74">
+        <f>Waggalitterfall!J22/10</f>
+        <v>3.9375</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75" s="3">
+        <v>34148</v>
+      </c>
+      <c r="C75">
+        <v>1.9959</v>
+      </c>
+      <c r="D75">
+        <f>WaggaBiomass!F23/10</f>
+        <v>452.9</v>
+      </c>
+      <c r="E75">
+        <f>WaggaBiomass!G23/10</f>
+        <v>1138.3</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="3"/>
+        <v>1591.1999999999998</v>
+      </c>
+      <c r="J75" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="K75">
+        <f>Waggalitterfall!J23/10</f>
+        <v>3.2549999999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76" t="s">
+        <v>66</v>
+      </c>
+      <c r="B76" s="3">
+        <v>34180</v>
+      </c>
+      <c r="C76">
+        <v>2.0821999999999998</v>
+      </c>
+      <c r="D76">
+        <f>WaggaBiomass!F24/10</f>
+        <v>484</v>
+      </c>
+      <c r="E76">
+        <f>WaggaBiomass!G24/10</f>
+        <v>1201</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="3"/>
+        <v>1685</v>
+      </c>
+      <c r="J76" s="4">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="K76">
+        <f>Waggalitterfall!J24/10</f>
+        <v>2.5912500000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77" t="s">
+        <v>66</v>
+      </c>
+      <c r="B77" s="3">
+        <v>34210</v>
+      </c>
+      <c r="C77">
+        <v>2.1671</v>
+      </c>
+      <c r="D77">
+        <f>WaggaBiomass!F25/10</f>
+        <v>486.7</v>
+      </c>
+      <c r="E77">
+        <f>WaggaBiomass!G25/10</f>
+        <v>1331.9</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="3"/>
+        <v>1818.6000000000001</v>
+      </c>
+      <c r="J77" s="4">
+        <v>5.2</v>
+      </c>
+      <c r="K77">
+        <f>Waggalitterfall!J25/10</f>
+        <v>4.7249999999999996</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78" t="s">
+        <v>66</v>
+      </c>
+      <c r="B78" s="3">
+        <v>34240</v>
+      </c>
+      <c r="C78">
+        <v>2.2492999999999999</v>
+      </c>
+      <c r="D78">
+        <f>WaggaBiomass!F26/10</f>
+        <v>492.2</v>
+      </c>
+      <c r="E78">
+        <f>WaggaBiomass!G26/10</f>
+        <v>1462.8</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="3"/>
+        <v>1955</v>
+      </c>
+      <c r="J78" s="4">
+        <v>5.4</v>
+      </c>
+      <c r="K78">
+        <f>Waggalitterfall!J26/10</f>
+        <v>9.7912499999999998</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79" t="s">
+        <v>66</v>
+      </c>
+      <c r="B79" s="3">
+        <v>34271</v>
+      </c>
+      <c r="C79">
+        <v>2.3342000000000001</v>
+      </c>
+      <c r="D79">
+        <f>WaggaBiomass!F27/10</f>
+        <v>503.1</v>
+      </c>
+      <c r="E79">
+        <f>WaggaBiomass!G27/10</f>
+        <v>1649.8</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="3"/>
+        <v>2152.9</v>
+      </c>
+      <c r="J79" s="4">
+        <v>5.7</v>
+      </c>
+      <c r="K79">
+        <f>Waggalitterfall!J27/10</f>
+        <v>22.162500000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80" t="s">
+        <v>66</v>
+      </c>
+      <c r="B80" s="3">
+        <v>34301</v>
+      </c>
+      <c r="C80">
+        <v>2.4163999999999999</v>
+      </c>
+      <c r="D80">
+        <f>WaggaBiomass!F28/10</f>
+        <v>526.79999999999995</v>
+      </c>
+      <c r="E80">
+        <f>WaggaBiomass!G28/10</f>
+        <v>1878</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="3"/>
+        <v>2404.8000000000002</v>
+      </c>
+      <c r="J80" s="4">
+        <v>5.9</v>
+      </c>
+      <c r="K80">
+        <f>Waggalitterfall!J28/10</f>
+        <v>61.645000000000003</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11">
+      <c r="A81" t="s">
+        <v>66</v>
+      </c>
+      <c r="B81" s="3">
+        <v>34333</v>
+      </c>
+      <c r="C81">
+        <v>2.5013999999999998</v>
+      </c>
+      <c r="D81">
+        <f>WaggaBiomass!F29/10</f>
+        <v>558.5</v>
+      </c>
+      <c r="E81">
+        <f>WaggaBiomass!G29/10</f>
+        <v>2184.1</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="3"/>
+        <v>2742.6</v>
+      </c>
+      <c r="J81" s="4">
+        <v>6.2</v>
+      </c>
+      <c r="K81">
+        <f>Waggalitterfall!J29/10</f>
+        <v>92.452500000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11">
+      <c r="A82" t="s">
+        <v>66</v>
+      </c>
+      <c r="B82" s="3">
+        <v>34363</v>
+      </c>
+      <c r="C82">
+        <v>2.5863</v>
+      </c>
+      <c r="D82">
+        <f>WaggaBiomass!F30/10</f>
+        <v>590</v>
+      </c>
+      <c r="E82">
+        <f>WaggaBiomass!G30/10</f>
+        <v>2538</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="3"/>
+        <v>3128</v>
+      </c>
+      <c r="J82" s="4">
+        <v>6.4</v>
+      </c>
+      <c r="K82">
+        <f>Waggalitterfall!J30/10</f>
+        <v>93.298749999999998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11">
+      <c r="A83" t="s">
+        <v>66</v>
+      </c>
+      <c r="B83" s="3">
+        <v>34391</v>
+      </c>
+      <c r="C83">
+        <v>2.6629999999999998</v>
+      </c>
+      <c r="D83">
+        <f>WaggaBiomass!F31/10</f>
+        <v>611</v>
+      </c>
+      <c r="E83">
+        <f>WaggaBiomass!G31/10</f>
+        <v>2806.3</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="3"/>
+        <v>3417.3</v>
+      </c>
+      <c r="J83" s="4">
+        <v>6.3</v>
+      </c>
+      <c r="K83">
+        <f>Waggalitterfall!J31/10</f>
+        <v>72.283749999999998</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11">
+      <c r="A84" t="s">
+        <v>66</v>
+      </c>
+      <c r="B84" s="3">
+        <v>34422</v>
+      </c>
+      <c r="C84">
+        <v>2.7479</v>
+      </c>
+      <c r="D84">
+        <f>WaggaBiomass!F32/10</f>
+        <v>623.20000000000005</v>
+      </c>
+      <c r="E84">
+        <f>WaggaBiomass!G32/10</f>
+        <v>3086</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="3"/>
+        <v>3709.2</v>
+      </c>
+      <c r="J84" s="4">
+        <v>6.2</v>
+      </c>
+      <c r="K84">
+        <f>Waggalitterfall!J32/10</f>
+        <v>40.366250000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11">
+      <c r="A85" t="s">
+        <v>66</v>
+      </c>
+      <c r="B85" s="3">
+        <v>34452</v>
+      </c>
+      <c r="C85">
+        <v>2.8300999999999998</v>
+      </c>
+      <c r="D85">
+        <f>WaggaBiomass!F33/10</f>
+        <v>632</v>
+      </c>
+      <c r="E85">
+        <f>WaggaBiomass!G33/10</f>
+        <v>3311</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="3"/>
+        <v>3943</v>
+      </c>
+      <c r="J85" s="4">
+        <v>6</v>
+      </c>
+      <c r="K85">
+        <f>Waggalitterfall!J33/10</f>
+        <v>32.152499999999996</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11">
+      <c r="A86" t="s">
+        <v>66</v>
+      </c>
+      <c r="B86" s="3">
+        <v>34484</v>
+      </c>
+      <c r="C86">
+        <v>2.9150999999999998</v>
+      </c>
+      <c r="D86">
+        <f>WaggaBiomass!F34/10</f>
+        <v>638</v>
+      </c>
+      <c r="E86">
+        <f>WaggaBiomass!G34/10</f>
+        <v>3479.5</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="3"/>
+        <v>4117.5</v>
+      </c>
+      <c r="J86" s="4">
+        <v>5.9</v>
+      </c>
+      <c r="K86">
+        <f>Waggalitterfall!J34/10</f>
+        <v>21.231249999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11">
+      <c r="A87" t="s">
+        <v>66</v>
+      </c>
+      <c r="B87" s="3">
+        <v>34514</v>
+      </c>
+      <c r="C87">
+        <v>2.9973000000000001</v>
+      </c>
+      <c r="D87">
+        <f>WaggaBiomass!F35/10</f>
+        <v>640.4</v>
+      </c>
+      <c r="E87">
+        <f>WaggaBiomass!G35/10</f>
+        <v>3607.4</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="3"/>
+        <v>4247.8</v>
+      </c>
+      <c r="J87" s="4">
+        <v>5.8</v>
+      </c>
+      <c r="K87">
+        <f>Waggalitterfall!J35/10</f>
+        <v>10.0175</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11">
+      <c r="A88" t="s">
+        <v>66</v>
+      </c>
+      <c r="B88" s="3">
+        <v>34545</v>
+      </c>
+      <c r="C88">
+        <v>3.0821999999999998</v>
+      </c>
+      <c r="D88">
+        <f>WaggaBiomass!F36/10</f>
+        <v>642</v>
+      </c>
+      <c r="E88">
+        <f>WaggaBiomass!G36/10</f>
+        <v>3695</v>
+      </c>
+      <c r="F88">
+        <f t="shared" si="3"/>
+        <v>4337</v>
+      </c>
+      <c r="J88" s="4">
+        <v>5.6</v>
+      </c>
+      <c r="K88">
+        <f>Waggalitterfall!J36/10</f>
+        <v>6.3562500000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11">
+      <c r="A89" t="s">
+        <v>66</v>
+      </c>
+      <c r="B89" s="3">
+        <v>34575</v>
+      </c>
+      <c r="C89">
+        <v>3.1671</v>
+      </c>
+      <c r="D89">
+        <f>WaggaBiomass!F37/10</f>
+        <v>642.5</v>
+      </c>
+      <c r="E89">
+        <f>WaggaBiomass!G37/10</f>
+        <v>3807</v>
+      </c>
+      <c r="F89">
+        <f t="shared" si="3"/>
+        <v>4449.5</v>
+      </c>
+      <c r="J89" s="4">
+        <v>5.6</v>
+      </c>
+      <c r="K89">
+        <f>Waggalitterfall!J37/10</f>
+        <v>15.508750000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11">
+      <c r="A90" t="s">
+        <v>66</v>
+      </c>
+      <c r="B90" s="3">
+        <v>34605</v>
+      </c>
+      <c r="C90">
+        <v>3.2492999999999999</v>
+      </c>
+      <c r="D90">
+        <f>WaggaBiomass!F38/10</f>
+        <v>643.20000000000005</v>
+      </c>
+      <c r="E90">
+        <f>WaggaBiomass!G38/10</f>
+        <v>3921.9</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="3"/>
+        <v>4565.1000000000004</v>
+      </c>
+      <c r="J90" s="4">
+        <v>5.7</v>
+      </c>
+      <c r="K90">
+        <f>Waggalitterfall!J38/10</f>
+        <v>21.963749999999997</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11">
+      <c r="A91" t="s">
+        <v>66</v>
+      </c>
+      <c r="B91" s="3">
+        <v>34636</v>
+      </c>
+      <c r="C91">
+        <v>3.3342000000000001</v>
+      </c>
+      <c r="D91">
+        <f>WaggaBiomass!F39/10</f>
+        <v>645.29999999999995</v>
+      </c>
+      <c r="E91">
+        <f>WaggaBiomass!G39/10</f>
+        <v>4085.6</v>
+      </c>
+      <c r="F91">
+        <f t="shared" si="3"/>
+        <v>4730.8999999999996</v>
+      </c>
+      <c r="J91" s="4">
+        <v>5.8</v>
+      </c>
+      <c r="K91">
+        <f>Waggalitterfall!J39/10</f>
+        <v>42.075000000000003</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11">
+      <c r="A92" t="s">
+        <v>66</v>
+      </c>
+      <c r="B92" s="3">
+        <v>34666</v>
+      </c>
+      <c r="C92">
+        <v>3.4163999999999999</v>
+      </c>
+      <c r="D92">
+        <f>WaggaBiomass!F40/10</f>
+        <v>648.9</v>
+      </c>
+      <c r="E92">
+        <f>WaggaBiomass!G40/10</f>
+        <v>4283.8</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="3"/>
+        <v>4932.7</v>
+      </c>
+      <c r="J92" s="4">
+        <v>5.9</v>
+      </c>
+      <c r="K92">
+        <f>Waggalitterfall!J40/10</f>
+        <v>66.027500000000003</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11">
+      <c r="A93" t="s">
+        <v>66</v>
+      </c>
+      <c r="B93" s="3">
+        <v>34698</v>
+      </c>
+      <c r="C93">
+        <v>3.5013999999999998</v>
+      </c>
+      <c r="D93">
+        <f>WaggaBiomass!F41/10</f>
+        <v>656.5</v>
+      </c>
+      <c r="E93">
+        <f>WaggaBiomass!G41/10</f>
+        <v>4550.8999999999996</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="3"/>
+        <v>5207.3999999999996</v>
+      </c>
+      <c r="J93" s="4">
+        <v>6.1</v>
+      </c>
+      <c r="K93">
+        <f>Waggalitterfall!J41/10</f>
+        <v>133.84375000000003</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11">
+      <c r="A94" t="s">
+        <v>66</v>
+      </c>
+      <c r="B94" s="3">
+        <v>34728</v>
+      </c>
+      <c r="C94">
+        <v>3.5863</v>
+      </c>
+      <c r="D94">
+        <f>WaggaBiomass!F42/10</f>
+        <v>659.6</v>
+      </c>
+      <c r="E94">
+        <f>WaggaBiomass!G42/10</f>
+        <v>4858.2</v>
+      </c>
+      <c r="F94">
+        <f t="shared" si="3"/>
+        <v>5517.8</v>
+      </c>
+      <c r="J94" s="4">
+        <v>6.2</v>
+      </c>
+      <c r="K94">
+        <f>Waggalitterfall!J42/10</f>
+        <v>54.839999999999996</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11">
+      <c r="A95" t="s">
+        <v>66</v>
+      </c>
+      <c r="B95" s="3">
+        <v>34756</v>
+      </c>
+      <c r="C95">
+        <v>3.6629999999999998</v>
+      </c>
+      <c r="D95">
+        <f>WaggaBiomass!F43/10</f>
+        <v>661.4</v>
+      </c>
+      <c r="E95">
+        <f>WaggaBiomass!G43/10</f>
+        <v>5254.5</v>
+      </c>
+      <c r="F95">
+        <f t="shared" si="3"/>
+        <v>5915.9</v>
+      </c>
+      <c r="J95" s="4">
+        <v>6.4</v>
+      </c>
+      <c r="K95">
+        <f>Waggalitterfall!J43/10</f>
+        <v>37.716250000000002</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11">
+      <c r="A96" t="s">
+        <v>66</v>
+      </c>
+      <c r="B96" s="3">
+        <v>34787</v>
+      </c>
+      <c r="C96">
+        <v>3.7479</v>
+      </c>
+      <c r="D96">
+        <f>WaggaBiomass!F44/10</f>
+        <v>666</v>
+      </c>
+      <c r="E96">
+        <f>WaggaBiomass!G44/10</f>
+        <v>5668.1</v>
+      </c>
+      <c r="F96">
+        <f t="shared" si="3"/>
+        <v>6334.1</v>
+      </c>
+      <c r="J96" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="K96">
+        <f>Waggalitterfall!J44/10</f>
+        <v>65.504999999999995</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11">
+      <c r="A97" t="s">
+        <v>66</v>
+      </c>
+      <c r="B97" s="3">
+        <v>34817</v>
+      </c>
+      <c r="C97">
+        <v>3.8300999999999998</v>
+      </c>
+      <c r="D97">
+        <f>WaggaBiomass!F45/10</f>
+        <v>667.7</v>
+      </c>
+      <c r="E97">
+        <f>WaggaBiomass!G45/10</f>
+        <v>5998.3</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="3"/>
+        <v>6666</v>
+      </c>
+      <c r="J97" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="K97">
+        <f>Waggalitterfall!J45/10</f>
+        <v>25.9925</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11">
+      <c r="A98" t="s">
+        <v>66</v>
+      </c>
+      <c r="B98" s="3">
+        <v>34849</v>
+      </c>
+      <c r="C98">
+        <v>3.9150999999999998</v>
+      </c>
+      <c r="D98">
+        <f>WaggaBiomass!F46/10</f>
+        <v>669.1</v>
+      </c>
+      <c r="E98">
+        <f>WaggaBiomass!G46/10</f>
+        <v>6245.3</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="3"/>
+        <v>6914.4000000000005</v>
+      </c>
+      <c r="J98" s="4">
+        <v>6.6</v>
+      </c>
+      <c r="K98">
+        <f>Waggalitterfall!J46/10</f>
+        <v>20.493749999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
+      <c r="A99" t="s">
+        <v>66</v>
+      </c>
+      <c r="B99" s="3">
+        <v>34879</v>
+      </c>
+      <c r="C99">
+        <v>3.9973000000000001</v>
+      </c>
+      <c r="D99">
+        <f>WaggaBiomass!F47/10</f>
+        <v>669.7</v>
+      </c>
+      <c r="E99">
+        <f>WaggaBiomass!G47/10</f>
+        <v>6434.9</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="3"/>
+        <v>7104.5999999999995</v>
+      </c>
+      <c r="J99" s="4">
+        <v>6.6</v>
+      </c>
+      <c r="K99">
+        <f>Waggalitterfall!J47/10</f>
+        <v>11.873749999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
+      <c r="A100" t="s">
+        <v>66</v>
+      </c>
+      <c r="B100" s="3">
+        <v>34910</v>
+      </c>
+      <c r="C100">
+        <v>4.0822000000000003</v>
+      </c>
+      <c r="D100">
+        <f>WaggaBiomass!F48/10</f>
+        <v>670</v>
+      </c>
+      <c r="E100">
+        <f>WaggaBiomass!G48/10</f>
+        <v>6567</v>
+      </c>
+      <c r="F100">
+        <f t="shared" si="3"/>
+        <v>7237</v>
+      </c>
+      <c r="J100" s="4">
+        <v>6.6</v>
+      </c>
+      <c r="K100">
+        <f>Waggalitterfall!J48/10</f>
+        <v>5.2562499999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>